<commit_message>
Improved basal area increment. Increment at t7 still incorrect
</commit_message>
<xml_diff>
--- a/out/yield_output.xlsx
+++ b/out/yield_output.xlsx
@@ -848,22 +848,22 @@
         <v>5000</v>
       </c>
       <c r="F14" t="n">
-        <v>4.19860926149098</v>
+        <v>3.60715613033392</v>
       </c>
       <c r="G14" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="H14" t="n">
         <v>5000</v>
       </c>
       <c r="I14" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="J14" t="n">
         <v>5.21703912077709</v>
       </c>
       <c r="K14" t="n">
-        <v>0</v>
+        <v>2.71848182305619</v>
       </c>
     </row>
     <row r="15">
@@ -883,16 +883,16 @@
         <v>5000</v>
       </c>
       <c r="F15" t="n">
-        <v>4.19860926149098</v>
+        <v>3.60715613033392</v>
       </c>
       <c r="G15" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="H15" t="n">
         <v>5000</v>
       </c>
       <c r="I15" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="J15" t="n">
         <v>5.70310512968476</v>
@@ -918,16 +918,16 @@
         <v>5000</v>
       </c>
       <c r="F16" t="n">
-        <v>4.19860926149098</v>
+        <v>3.60715613033392</v>
       </c>
       <c r="G16" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="H16" t="n">
         <v>5000</v>
       </c>
       <c r="I16" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="J16" t="n">
         <v>6.17749196461765</v>
@@ -953,16 +953,16 @@
         <v>5000</v>
       </c>
       <c r="F17" t="n">
-        <v>4.19860926149098</v>
+        <v>3.60715613033392</v>
       </c>
       <c r="G17" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="H17" t="n">
         <v>5000</v>
       </c>
       <c r="I17" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="J17" t="n">
         <v>6.64956270015096</v>
@@ -988,16 +988,16 @@
         <v>5000</v>
       </c>
       <c r="F18" t="n">
-        <v>4.19860926149098</v>
+        <v>3.60715613033392</v>
       </c>
       <c r="G18" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="H18" t="n">
         <v>5000</v>
       </c>
       <c r="I18" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="J18" t="n">
         <v>7.11850619468903</v>
@@ -1023,16 +1023,16 @@
         <v>5000</v>
       </c>
       <c r="F19" t="n">
-        <v>4.19860926149098</v>
+        <v>3.60715613033392</v>
       </c>
       <c r="G19" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="H19" t="n">
         <v>5000</v>
       </c>
       <c r="I19" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="J19" t="n">
         <v>7.58362514354308</v>
@@ -1058,16 +1058,16 @@
         <v>5000</v>
       </c>
       <c r="F20" t="n">
-        <v>4.19860926149098</v>
+        <v>3.60715613033392</v>
       </c>
       <c r="G20" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="H20" t="n">
         <v>5000</v>
       </c>
       <c r="I20" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="J20" t="n">
         <v>8.0443201514607</v>
@@ -1093,16 +1093,16 @@
         <v>5000</v>
       </c>
       <c r="F21" t="n">
-        <v>4.19860926149098</v>
+        <v>3.60715613033392</v>
       </c>
       <c r="G21" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="H21" t="n">
         <v>5000</v>
       </c>
       <c r="I21" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="J21" t="n">
         <v>8.50007657967768</v>
@@ -1128,16 +1128,16 @@
         <v>5000</v>
       </c>
       <c r="F22" t="n">
-        <v>4.19860926149098</v>
+        <v>3.60715613033392</v>
       </c>
       <c r="G22" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="H22" t="n">
         <v>5000</v>
       </c>
       <c r="I22" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="J22" t="n">
         <v>8.95045356445584</v>
@@ -1163,16 +1163,16 @@
         <v>5000</v>
       </c>
       <c r="F23" t="n">
-        <v>4.19860926149098</v>
+        <v>3.60715613033392</v>
       </c>
       <c r="G23" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="H23" t="n">
         <v>5000</v>
       </c>
       <c r="I23" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="J23" t="n">
         <v>9.39507475999458</v>
@@ -1198,16 +1198,16 @@
         <v>5000</v>
       </c>
       <c r="F24" t="n">
-        <v>4.19860926149098</v>
+        <v>3.60715613033392</v>
       </c>
       <c r="G24" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="H24" t="n">
         <v>5000</v>
       </c>
       <c r="I24" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="J24" t="n">
         <v>9.83362046849985</v>
@@ -1233,16 +1233,16 @@
         <v>5000</v>
       </c>
       <c r="F25" t="n">
-        <v>4.19860926149098</v>
+        <v>3.60715613033392</v>
       </c>
       <c r="G25" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="H25" t="n">
         <v>5000</v>
       </c>
       <c r="I25" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="J25" t="n">
         <v>10.2658208991482</v>
@@ -1268,16 +1268,16 @@
         <v>5000</v>
       </c>
       <c r="F26" t="n">
-        <v>4.19860926149098</v>
+        <v>3.60715613033392</v>
       </c>
       <c r="G26" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="H26" t="n">
         <v>5000</v>
       </c>
       <c r="I26" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="J26" t="n">
         <v>10.6914503553973</v>
@@ -1303,16 +1303,16 @@
         <v>5000</v>
       </c>
       <c r="F27" t="n">
-        <v>4.19860926149098</v>
+        <v>3.60715613033392</v>
       </c>
       <c r="G27" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="H27" t="n">
         <v>5000</v>
       </c>
       <c r="I27" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="J27" t="n">
         <v>11.1103221929444</v>
@@ -1338,16 +1338,16 @@
         <v>5000</v>
       </c>
       <c r="F28" t="n">
-        <v>4.19860926149098</v>
+        <v>3.60715613033392</v>
       </c>
       <c r="G28" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="H28" t="n">
         <v>5000</v>
       </c>
       <c r="I28" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="J28" t="n">
         <v>11.5222844229026</v>
@@ -1373,16 +1373,16 @@
         <v>5000</v>
       </c>
       <c r="F29" t="n">
-        <v>4.19860926149098</v>
+        <v>3.60715613033392</v>
       </c>
       <c r="G29" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="H29" t="n">
         <v>5000</v>
       </c>
       <c r="I29" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="J29" t="n">
         <v>11.9272158593845</v>
@@ -1408,16 +1408,16 @@
         <v>5000</v>
       </c>
       <c r="F30" t="n">
-        <v>4.19860926149098</v>
+        <v>3.60715613033392</v>
       </c>
       <c r="G30" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="H30" t="n">
         <v>5000</v>
       </c>
       <c r="I30" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="J30" t="n">
         <v>12.3250227296902</v>
@@ -1443,16 +1443,16 @@
         <v>5000</v>
       </c>
       <c r="F31" t="n">
-        <v>4.19860926149098</v>
+        <v>3.60715613033392</v>
       </c>
       <c r="G31" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="H31" t="n">
         <v>5000</v>
       </c>
       <c r="I31" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="J31" t="n">
         <v>12.7156356801296</v>
@@ -1478,16 +1478,16 @@
         <v>5000</v>
       </c>
       <c r="F32" t="n">
-        <v>4.19860926149098</v>
+        <v>3.60715613033392</v>
       </c>
       <c r="G32" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="H32" t="n">
         <v>5000</v>
       </c>
       <c r="I32" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="J32" t="n">
         <v>13.0990071222085</v>
@@ -1513,16 +1513,16 @@
         <v>5000</v>
       </c>
       <c r="F33" t="n">
-        <v>4.19860926149098</v>
+        <v>3.60715613033392</v>
       </c>
       <c r="G33" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="H33" t="n">
         <v>5000</v>
       </c>
       <c r="I33" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="J33" t="n">
         <v>13.475108873216</v>
@@ -1548,16 +1548,16 @@
         <v>5000</v>
       </c>
       <c r="F34" t="n">
-        <v>4.19860926149098</v>
+        <v>3.60715613033392</v>
       </c>
       <c r="G34" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="H34" t="n">
         <v>5000</v>
       </c>
       <c r="I34" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="J34" t="n">
         <v>13.8439300527273</v>
@@ -1583,16 +1583,16 @@
         <v>5000</v>
       </c>
       <c r="F35" t="n">
-        <v>4.19860926149098</v>
+        <v>3.60715613033392</v>
       </c>
       <c r="G35" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="H35" t="n">
         <v>5000</v>
       </c>
       <c r="I35" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="J35" t="n">
         <v>14.205475202582</v>
@@ -1618,16 +1618,16 @@
         <v>5000</v>
       </c>
       <c r="F36" t="n">
-        <v>4.19860926149098</v>
+        <v>3.60715613033392</v>
       </c>
       <c r="G36" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="H36" t="n">
         <v>5000</v>
       </c>
       <c r="I36" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="J36" t="n">
         <v>14.5597626028354</v>
@@ -1653,16 +1653,16 @@
         <v>5000</v>
       </c>
       <c r="F37" t="n">
-        <v>4.19860926149098</v>
+        <v>3.60715613033392</v>
       </c>
       <c r="G37" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="H37" t="n">
         <v>5000</v>
       </c>
       <c r="I37" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="J37" t="n">
         <v>14.9068227602292</v>
@@ -1688,16 +1688,16 @@
         <v>5000</v>
       </c>
       <c r="F38" t="n">
-        <v>4.19860926149098</v>
+        <v>3.60715613033392</v>
       </c>
       <c r="G38" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="H38" t="n">
         <v>5000</v>
       </c>
       <c r="I38" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="J38" t="n">
         <v>15.2466970490801</v>
@@ -1723,16 +1723,16 @@
         <v>5000</v>
       </c>
       <c r="F39" t="n">
-        <v>4.19860926149098</v>
+        <v>3.60715613033392</v>
       </c>
       <c r="G39" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="H39" t="n">
         <v>5000</v>
       </c>
       <c r="I39" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="J39" t="n">
         <v>15.5794364872729</v>
@@ -1758,16 +1758,16 @@
         <v>5000</v>
       </c>
       <c r="F40" t="n">
-        <v>4.19860926149098</v>
+        <v>3.60715613033392</v>
       </c>
       <c r="G40" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="H40" t="n">
         <v>5000</v>
       </c>
       <c r="I40" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="J40" t="n">
         <v>15.9051006323723</v>
@@ -1793,16 +1793,16 @@
         <v>5000</v>
       </c>
       <c r="F41" t="n">
-        <v>4.19860926149098</v>
+        <v>3.60715613033392</v>
       </c>
       <c r="G41" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="H41" t="n">
         <v>5000</v>
       </c>
       <c r="I41" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="J41" t="n">
         <v>16.2237565848382</v>
@@ -1828,16 +1828,16 @@
         <v>5000</v>
       </c>
       <c r="F42" t="n">
-        <v>4.19860926149098</v>
+        <v>3.60715613033392</v>
       </c>
       <c r="G42" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="H42" t="n">
         <v>5000</v>
       </c>
       <c r="I42" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="J42" t="n">
         <v>16.5354780869818</v>
@@ -1863,16 +1863,16 @@
         <v>5000</v>
       </c>
       <c r="F43" t="n">
-        <v>4.19860926149098</v>
+        <v>3.60715613033392</v>
       </c>
       <c r="G43" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="H43" t="n">
         <v>5000</v>
       </c>
       <c r="I43" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="J43" t="n">
         <v>16.8403447077157</v>
@@ -1898,16 +1898,16 @@
         <v>5000</v>
       </c>
       <c r="F44" t="n">
-        <v>4.19860926149098</v>
+        <v>3.60715613033392</v>
       </c>
       <c r="G44" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="H44" t="n">
         <v>5000</v>
       </c>
       <c r="I44" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="J44" t="n">
         <v>17.1384411043553</v>
@@ -1933,16 +1933,16 @@
         <v>5000</v>
       </c>
       <c r="F45" t="n">
-        <v>4.19860926149098</v>
+        <v>3.60715613033392</v>
       </c>
       <c r="G45" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="H45" t="n">
         <v>5000</v>
       </c>
       <c r="I45" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="J45" t="n">
         <v>17.4298563537614</v>
@@ -1968,16 +1968,16 @@
         <v>5000</v>
       </c>
       <c r="F46" t="n">
-        <v>4.19860926149098</v>
+        <v>3.60715613033392</v>
       </c>
       <c r="G46" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="H46" t="n">
         <v>5000</v>
       </c>
       <c r="I46" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="J46" t="n">
         <v>17.7146833460055</v>
@@ -2003,16 +2003,16 @@
         <v>5000</v>
       </c>
       <c r="F47" t="n">
-        <v>4.19860926149098</v>
+        <v>3.60715613033392</v>
       </c>
       <c r="G47" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="H47" t="n">
         <v>5000</v>
       </c>
       <c r="I47" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="J47" t="n">
         <v>17.993018234509</v>
@@ -2038,16 +2038,16 @@
         <v>5000</v>
       </c>
       <c r="F48" t="n">
-        <v>4.19860926149098</v>
+        <v>3.60715613033392</v>
       </c>
       <c r="G48" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="H48" t="n">
         <v>5000</v>
       </c>
       <c r="I48" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="J48" t="n">
         <v>18.2649599372746</v>
@@ -2073,16 +2073,16 @@
         <v>5000</v>
       </c>
       <c r="F49" t="n">
-        <v>4.19860926149098</v>
+        <v>3.60715613033392</v>
       </c>
       <c r="G49" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="H49" t="n">
         <v>5000</v>
       </c>
       <c r="I49" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="J49" t="n">
         <v>18.5306096844126</v>
@@ -2108,16 +2108,16 @@
         <v>5000</v>
       </c>
       <c r="F50" t="n">
-        <v>4.19860926149098</v>
+        <v>3.60715613033392</v>
       </c>
       <c r="G50" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="H50" t="n">
         <v>5000</v>
       </c>
       <c r="I50" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="J50" t="n">
         <v>18.7900706076699</v>
@@ -2143,16 +2143,16 @@
         <v>5000</v>
       </c>
       <c r="F51" t="n">
-        <v>4.19860926149098</v>
+        <v>3.60715613033392</v>
       </c>
       <c r="G51" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="H51" t="n">
         <v>5000</v>
       </c>
       <c r="I51" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="J51" t="n">
         <v>19.0434473681203</v>
@@ -2178,16 +2178,16 @@
         <v>5000</v>
       </c>
       <c r="F52" t="n">
-        <v>4.19860926149098</v>
+        <v>3.60715613033392</v>
       </c>
       <c r="G52" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="H52" t="n">
         <v>5000</v>
       </c>
       <c r="I52" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="J52" t="n">
         <v>19.290845818561</v>
@@ -2213,16 +2213,16 @@
         <v>5000</v>
       </c>
       <c r="F53" t="n">
-        <v>4.19860926149098</v>
+        <v>3.60715613033392</v>
       </c>
       <c r="G53" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="H53" t="n">
         <v>5000</v>
       </c>
       <c r="I53" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="J53" t="n">
         <v>19.5323726975124</v>
@@ -2248,16 +2248,16 @@
         <v>5000</v>
       </c>
       <c r="F54" t="n">
-        <v>4.19860926149098</v>
+        <v>3.60715613033392</v>
       </c>
       <c r="G54" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="H54" t="n">
         <v>5000</v>
       </c>
       <c r="I54" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="J54" t="n">
         <v>19.7681353520192</v>
@@ -2283,16 +2283,16 @@
         <v>5000</v>
       </c>
       <c r="F55" t="n">
-        <v>4.19860926149098</v>
+        <v>3.60715613033392</v>
       </c>
       <c r="G55" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="H55" t="n">
         <v>5000</v>
       </c>
       <c r="I55" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="J55" t="n">
         <v>19.9982414867245</v>
@@ -2318,16 +2318,16 @@
         <v>5000</v>
       </c>
       <c r="F56" t="n">
-        <v>4.19860926149098</v>
+        <v>3.60715613033392</v>
       </c>
       <c r="G56" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="H56" t="n">
         <v>5000</v>
       </c>
       <c r="I56" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="J56" t="n">
         <v>20.2227989369298</v>
@@ -2353,16 +2353,16 @@
         <v>5000</v>
       </c>
       <c r="F57" t="n">
-        <v>4.19860926149098</v>
+        <v>3.60715613033392</v>
       </c>
       <c r="G57" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="H57" t="n">
         <v>5000</v>
       </c>
       <c r="I57" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="J57" t="n">
         <v>20.4419154635675</v>
@@ -2388,16 +2388,16 @@
         <v>5000</v>
       </c>
       <c r="F58" t="n">
-        <v>4.19860926149098</v>
+        <v>3.60715613033392</v>
       </c>
       <c r="G58" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="H58" t="n">
         <v>5000</v>
       </c>
       <c r="I58" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="J58" t="n">
         <v>20.6556985682052</v>
@@ -2423,16 +2423,16 @@
         <v>5000</v>
       </c>
       <c r="F59" t="n">
-        <v>4.19860926149098</v>
+        <v>3.60715613033392</v>
       </c>
       <c r="G59" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="H59" t="n">
         <v>5000</v>
       </c>
       <c r="I59" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="J59" t="n">
         <v>20.8642553263727</v>
@@ -2458,16 +2458,16 @@
         <v>5000</v>
       </c>
       <c r="F60" t="n">
-        <v>4.19860926149098</v>
+        <v>3.60715613033392</v>
       </c>
       <c r="G60" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="H60" t="n">
         <v>5000</v>
       </c>
       <c r="I60" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="J60" t="n">
         <v>21.0676922376561</v>
@@ -2493,16 +2493,16 @@
         <v>5000</v>
       </c>
       <c r="F61" t="n">
-        <v>4.19860926149098</v>
+        <v>3.60715613033392</v>
       </c>
       <c r="G61" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="H61" t="n">
         <v>5000</v>
       </c>
       <c r="I61" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="J61" t="n">
         <v>21.2661150911433</v>
@@ -2528,16 +2528,16 @@
         <v>5000</v>
       </c>
       <c r="F62" t="n">
-        <v>4.19860926149098</v>
+        <v>3.60715613033392</v>
       </c>
       <c r="G62" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="H62" t="n">
         <v>5000</v>
       </c>
       <c r="I62" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="J62" t="n">
         <v>21.4596288449269</v>
@@ -2563,16 +2563,16 @@
         <v>5000</v>
       </c>
       <c r="F63" t="n">
-        <v>4.19860926149098</v>
+        <v>3.60715613033392</v>
       </c>
       <c r="G63" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="H63" t="n">
         <v>5000</v>
       </c>
       <c r="I63" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="J63" t="n">
         <v>21.6483375184856</v>
@@ -2598,16 +2598,16 @@
         <v>5000</v>
       </c>
       <c r="F64" t="n">
-        <v>4.19860926149098</v>
+        <v>3.60715613033392</v>
       </c>
       <c r="G64" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="H64" t="n">
         <v>5000</v>
       </c>
       <c r="I64" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="J64" t="n">
         <v>21.832344096866</v>
@@ -2633,16 +2633,16 @@
         <v>5000</v>
       </c>
       <c r="F65" t="n">
-        <v>4.19860926149098</v>
+        <v>3.60715613033392</v>
       </c>
       <c r="G65" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="H65" t="n">
         <v>5000</v>
       </c>
       <c r="I65" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="J65" t="n">
         <v>22.0117504456764</v>
@@ -2668,16 +2668,16 @@
         <v>5000</v>
       </c>
       <c r="F66" t="n">
-        <v>4.19860926149098</v>
+        <v>3.60715613033392</v>
       </c>
       <c r="G66" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="H66" t="n">
         <v>5000</v>
       </c>
       <c r="I66" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="J66" t="n">
         <v>22.1866572359911</v>
@@ -2703,16 +2703,16 @@
         <v>5000</v>
       </c>
       <c r="F67" t="n">
-        <v>4.19860926149098</v>
+        <v>3.60715613033392</v>
       </c>
       <c r="G67" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="H67" t="n">
         <v>5000</v>
       </c>
       <c r="I67" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="J67" t="n">
         <v>22.3571638783349</v>
@@ -2738,16 +2738,16 @@
         <v>5000</v>
       </c>
       <c r="F68" t="n">
-        <v>4.19860926149098</v>
+        <v>3.60715613033392</v>
       </c>
       <c r="G68" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="H68" t="n">
         <v>5000</v>
       </c>
       <c r="I68" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="J68" t="n">
         <v>22.5233684649905</v>
@@ -2773,16 +2773,16 @@
         <v>5000</v>
       </c>
       <c r="F69" t="n">
-        <v>4.19860926149098</v>
+        <v>3.60715613033392</v>
       </c>
       <c r="G69" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="H69" t="n">
         <v>5000</v>
       </c>
       <c r="I69" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="J69" t="n">
         <v>22.6853677199294</v>
@@ -2808,16 +2808,16 @@
         <v>5000</v>
       </c>
       <c r="F70" t="n">
-        <v>4.19860926149098</v>
+        <v>3.60715613033392</v>
       </c>
       <c r="G70" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="H70" t="n">
         <v>5000</v>
       </c>
       <c r="I70" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="J70" t="n">
         <v>22.8432569557282</v>
@@ -2843,16 +2843,16 @@
         <v>5000</v>
       </c>
       <c r="F71" t="n">
-        <v>4.19860926149098</v>
+        <v>3.60715613033392</v>
       </c>
       <c r="G71" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="H71" t="n">
         <v>5000</v>
       </c>
       <c r="I71" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="J71" t="n">
         <v>22.9971300368802</v>
@@ -2878,16 +2878,16 @@
         <v>5000</v>
       </c>
       <c r="F72" t="n">
-        <v>4.19860926149098</v>
+        <v>3.60715613033392</v>
       </c>
       <c r="G72" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="H72" t="n">
         <v>5000</v>
       </c>
       <c r="I72" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="J72" t="n">
         <v>23.1470793489612</v>
@@ -2913,16 +2913,16 @@
         <v>5000</v>
       </c>
       <c r="F73" t="n">
-        <v>4.19860926149098</v>
+        <v>3.60715613033392</v>
       </c>
       <c r="G73" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="H73" t="n">
         <v>5000</v>
       </c>
       <c r="I73" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="J73" t="n">
         <v>23.2931957731536</v>
@@ -2948,16 +2948,16 @@
         <v>5000</v>
       </c>
       <c r="F74" t="n">
-        <v>4.19860926149098</v>
+        <v>3.60715613033392</v>
       </c>
       <c r="G74" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="H74" t="n">
         <v>5000</v>
       </c>
       <c r="I74" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="J74" t="n">
         <v>23.4355686656674</v>
@@ -2983,16 +2983,16 @@
         <v>5000</v>
       </c>
       <c r="F75" t="n">
-        <v>4.19860926149098</v>
+        <v>3.60715613033392</v>
       </c>
       <c r="G75" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="H75" t="n">
         <v>5000</v>
       </c>
       <c r="I75" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="J75" t="n">
         <v>23.5742858416393</v>
@@ -3018,16 +3018,16 @@
         <v>5000</v>
       </c>
       <c r="F76" t="n">
-        <v>4.19860926149098</v>
+        <v>3.60715613033392</v>
       </c>
       <c r="G76" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="H76" t="n">
         <v>5000</v>
       </c>
       <c r="I76" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="J76" t="n">
         <v>23.7094335631191</v>
@@ -3053,16 +3053,16 @@
         <v>5000</v>
       </c>
       <c r="F77" t="n">
-        <v>4.19860926149098</v>
+        <v>3.60715613033392</v>
       </c>
       <c r="G77" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="H77" t="n">
         <v>5000</v>
       </c>
       <c r="I77" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="J77" t="n">
         <v>23.8410965307854</v>
@@ -3088,16 +3088,16 @@
         <v>5000</v>
       </c>
       <c r="F78" t="n">
-        <v>4.19860926149098</v>
+        <v>3.60715613033392</v>
       </c>
       <c r="G78" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="H78" t="n">
         <v>5000</v>
       </c>
       <c r="I78" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="J78" t="n">
         <v>23.9693578790612</v>
@@ -3123,16 +3123,16 @@
         <v>5000</v>
       </c>
       <c r="F79" t="n">
-        <v>4.19860926149098</v>
+        <v>3.60715613033392</v>
       </c>
       <c r="G79" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="H79" t="n">
         <v>5000</v>
       </c>
       <c r="I79" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="J79" t="n">
         <v>24.0942991743251</v>
@@ -3158,16 +3158,16 @@
         <v>5000</v>
       </c>
       <c r="F80" t="n">
-        <v>4.19860926149098</v>
+        <v>3.60715613033392</v>
       </c>
       <c r="G80" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="H80" t="n">
         <v>5000</v>
       </c>
       <c r="I80" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="J80" t="n">
         <v>24.2160004159351</v>
@@ -3193,16 +3193,16 @@
         <v>5000</v>
       </c>
       <c r="F81" t="n">
-        <v>4.19860926149098</v>
+        <v>3.60715613033392</v>
       </c>
       <c r="G81" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="H81" t="n">
         <v>5000</v>
       </c>
       <c r="I81" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="J81" t="n">
         <v>24.3345400398095</v>
@@ -3228,16 +3228,16 @@
         <v>5000</v>
       </c>
       <c r="F82" t="n">
-        <v>4.19860926149098</v>
+        <v>3.60715613033392</v>
       </c>
       <c r="G82" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="H82" t="n">
         <v>5000</v>
       </c>
       <c r="I82" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="J82" t="n">
         <v>24.4499949243228</v>
@@ -3263,16 +3263,16 @@
         <v>5000</v>
       </c>
       <c r="F83" t="n">
-        <v>4.19860926149098</v>
+        <v>3.60715613033392</v>
       </c>
       <c r="G83" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="H83" t="n">
         <v>5000</v>
       </c>
       <c r="I83" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="J83" t="n">
         <v>24.5624403982984</v>
@@ -3298,16 +3298,16 @@
         <v>5000</v>
       </c>
       <c r="F84" t="n">
-        <v>4.19860926149098</v>
+        <v>3.60715613033392</v>
       </c>
       <c r="G84" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="H84" t="n">
         <v>5000</v>
       </c>
       <c r="I84" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="J84" t="n">
         <v>24.6719502508934</v>
@@ -3333,16 +3333,16 @@
         <v>5000</v>
       </c>
       <c r="F85" t="n">
-        <v>4.19860926149098</v>
+        <v>3.60715613033392</v>
       </c>
       <c r="G85" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="H85" t="n">
         <v>5000</v>
       </c>
       <c r="I85" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="J85" t="n">
         <v>24.778596743189</v>
@@ -3368,16 +3368,16 @@
         <v>5000</v>
       </c>
       <c r="F86" t="n">
-        <v>4.19860926149098</v>
+        <v>3.60715613033392</v>
       </c>
       <c r="G86" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="H86" t="n">
         <v>5000</v>
       </c>
       <c r="I86" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="J86" t="n">
         <v>24.8824506213118</v>
@@ -3403,16 +3403,16 @@
         <v>5000</v>
       </c>
       <c r="F87" t="n">
-        <v>4.19860926149098</v>
+        <v>3.60715613033392</v>
       </c>
       <c r="G87" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="H87" t="n">
         <v>5000</v>
       </c>
       <c r="I87" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="J87" t="n">
         <v>24.9835811309291</v>
@@ -3438,16 +3438,16 @@
         <v>5000</v>
       </c>
       <c r="F88" t="n">
-        <v>4.19860926149098</v>
+        <v>3.60715613033392</v>
       </c>
       <c r="G88" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="H88" t="n">
         <v>5000</v>
       </c>
       <c r="I88" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="J88" t="n">
         <v>25.0820560329676</v>
@@ -3473,16 +3473,16 @@
         <v>5000</v>
       </c>
       <c r="F89" t="n">
-        <v>4.19860926149098</v>
+        <v>3.60715613033392</v>
       </c>
       <c r="G89" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="H89" t="n">
         <v>5000</v>
       </c>
       <c r="I89" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="J89" t="n">
         <v>25.1779416204226</v>
@@ -3508,16 +3508,16 @@
         <v>5000</v>
       </c>
       <c r="F90" t="n">
-        <v>4.19860926149098</v>
+        <v>3.60715613033392</v>
       </c>
       <c r="G90" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="H90" t="n">
         <v>5000</v>
       </c>
       <c r="I90" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="J90" t="n">
         <v>25.2713027361307</v>
@@ -3543,16 +3543,16 @@
         <v>5000</v>
       </c>
       <c r="F91" t="n">
-        <v>4.19860926149098</v>
+        <v>3.60715613033392</v>
       </c>
       <c r="G91" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="H91" t="n">
         <v>5000</v>
       </c>
       <c r="I91" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="J91" t="n">
         <v>25.3622027913914</v>
@@ -3578,16 +3578,16 @@
         <v>5000</v>
       </c>
       <c r="F92" t="n">
-        <v>4.19860926149098</v>
+        <v>3.60715613033392</v>
       </c>
       <c r="G92" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="H92" t="n">
         <v>5000</v>
       </c>
       <c r="I92" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="J92" t="n">
         <v>25.4507037853313</v>
@@ -3613,16 +3613,16 @@
         <v>5000</v>
       </c>
       <c r="F93" t="n">
-        <v>4.19860926149098</v>
+        <v>3.60715613033392</v>
       </c>
       <c r="G93" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="H93" t="n">
         <v>5000</v>
       </c>
       <c r="I93" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="J93" t="n">
         <v>25.5368663249128</v>
@@ -3648,16 +3648,16 @@
         <v>5000</v>
       </c>
       <c r="F94" t="n">
-        <v>4.19860926149098</v>
+        <v>3.60715613033392</v>
       </c>
       <c r="G94" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="H94" t="n">
         <v>5000</v>
       </c>
       <c r="I94" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="J94" t="n">
         <v>25.6207496454972</v>
@@ -3683,16 +3683,16 @@
         <v>5000</v>
       </c>
       <c r="F95" t="n">
-        <v>4.19860926149098</v>
+        <v>3.60715613033392</v>
       </c>
       <c r="G95" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="H95" t="n">
         <v>5000</v>
       </c>
       <c r="I95" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="J95" t="n">
         <v>25.702411631879</v>
@@ -3718,16 +3718,16 @@
         <v>5000</v>
       </c>
       <c r="F96" t="n">
-        <v>4.19860926149098</v>
+        <v>3.60715613033392</v>
       </c>
       <c r="G96" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="H96" t="n">
         <v>5000</v>
       </c>
       <c r="I96" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="J96" t="n">
         <v>25.7819088397162</v>
@@ -3753,16 +3753,16 @@
         <v>5000</v>
       </c>
       <c r="F97" t="n">
-        <v>4.19860926149098</v>
+        <v>3.60715613033392</v>
       </c>
       <c r="G97" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="H97" t="n">
         <v>5000</v>
       </c>
       <c r="I97" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="J97" t="n">
         <v>25.859296517285</v>
@@ -3788,16 +3788,16 @@
         <v>5000</v>
       </c>
       <c r="F98" t="n">
-        <v>4.19860926149098</v>
+        <v>3.60715613033392</v>
       </c>
       <c r="G98" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="H98" t="n">
         <v>5000</v>
       </c>
       <c r="I98" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="J98" t="n">
         <v>25.9346286274961</v>
@@ -3823,16 +3823,16 @@
         <v>5000</v>
       </c>
       <c r="F99" t="n">
-        <v>4.19860926149098</v>
+        <v>3.60715613033392</v>
       </c>
       <c r="G99" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="H99" t="n">
         <v>5000</v>
       </c>
       <c r="I99" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="J99" t="n">
         <v>26.007957870112</v>
@@ -3858,16 +3858,16 @@
         <v>5000</v>
       </c>
       <c r="F100" t="n">
-        <v>4.19860926149098</v>
+        <v>3.60715613033392</v>
       </c>
       <c r="G100" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="H100" t="n">
         <v>5000</v>
       </c>
       <c r="I100" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="J100" t="n">
         <v>26.0793357041125</v>
@@ -3893,16 +3893,16 @@
         <v>5000</v>
       </c>
       <c r="F101" t="n">
-        <v>4.19860926149098</v>
+        <v>3.60715613033392</v>
       </c>
       <c r="G101" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="H101" t="n">
         <v>5000</v>
       </c>
       <c r="I101" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="J101" t="n">
         <v>26.1488123701586</v>
@@ -3928,16 +3928,16 @@
         <v>5000</v>
       </c>
       <c r="F102" t="n">
-        <v>4.19860926149098</v>
+        <v>3.60715613033392</v>
       </c>
       <c r="G102" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="H102" t="n">
         <v>5000</v>
       </c>
       <c r="I102" t="n">
-        <v>6.92262497012867</v>
+        <v>5.10963369085116</v>
       </c>
       <c r="J102" t="n">
         <v>26.2164369131087</v>

</xml_diff>

<commit_message>
Stem number changes due to thinning added
</commit_message>
<xml_diff>
--- a/out/yield_output.xlsx
+++ b/out/yield_output.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t xml:space="preserve">t</t>
   </si>
@@ -45,6 +45,9 @@
   </si>
   <si>
     <t xml:space="preserve">ic_g</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n_th</t>
   </si>
 </sst>
 </file>
@@ -410,13 +413,16 @@
       <c r="K1" t="s">
         <v>10</v>
       </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>16</v>
+        <v>679409451580235</v>
       </c>
       <c r="C2" t="n">
         <v>0.000000000000223675349847527</v>
@@ -445,13 +451,14 @@
       <c r="K2" t="n">
         <v>0</v>
       </c>
+      <c r="L2"/>
     </row>
     <row r="3">
       <c r="A3" t="n">
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>16</v>
+        <v>1859156.75523231</v>
       </c>
       <c r="C3" t="n">
         <v>0.0000817398244361254</v>
@@ -480,13 +487,14 @@
       <c r="K3" t="n">
         <v>0</v>
       </c>
+      <c r="L3"/>
     </row>
     <row r="4">
       <c r="A4" t="n">
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>16</v>
+        <v>9757.73786644576</v>
       </c>
       <c r="C4" t="n">
         <v>0.015574014064725</v>
@@ -515,13 +523,14 @@
       <c r="K4" t="n">
         <v>0</v>
       </c>
+      <c r="L4"/>
     </row>
     <row r="5">
       <c r="A5" t="n">
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>16</v>
+        <v>989.970577781789</v>
       </c>
       <c r="C5" t="n">
         <v>0.153506730586313</v>
@@ -550,13 +559,14 @@
       <c r="K5" t="n">
         <v>0</v>
       </c>
+      <c r="L5"/>
     </row>
     <row r="6">
       <c r="A6" t="n">
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>16</v>
+        <v>285.895865312284</v>
       </c>
       <c r="C6" t="n">
         <v>0.531547200257451</v>
@@ -585,13 +595,14 @@
       <c r="K6" t="n">
         <v>0</v>
       </c>
+      <c r="L6"/>
     </row>
     <row r="7">
       <c r="A7" t="n">
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>16</v>
+        <v>133.032122735235</v>
       </c>
       <c r="C7" t="n">
         <v>1.14233422460209</v>
@@ -620,13 +631,14 @@
       <c r="K7" t="n">
         <v>0</v>
       </c>
+      <c r="L7"/>
     </row>
     <row r="8">
       <c r="A8" t="n">
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>16</v>
+        <v>79.7407925629862</v>
       </c>
       <c r="C8" t="n">
         <v>1.90576418778242</v>
@@ -655,13 +667,14 @@
       <c r="K8" t="n">
         <v>0</v>
       </c>
+      <c r="L8"/>
     </row>
     <row r="9">
       <c r="A9" t="n">
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>16</v>
+        <v>55.4676458479483</v>
       </c>
       <c r="C9" t="n">
         <v>2.73974394349651</v>
@@ -690,13 +703,14 @@
       <c r="K9" t="n">
         <v>0</v>
       </c>
+      <c r="L9"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>16</v>
+        <v>42.3906620388109</v>
       </c>
       <c r="C10" t="n">
         <v>3.58492034478706</v>
@@ -725,13 +739,14 @@
       <c r="K10" t="n">
         <v>0</v>
       </c>
+      <c r="L10"/>
     </row>
     <row r="11">
       <c r="A11" t="n">
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>16</v>
+        <v>34.4995521177324</v>
       </c>
       <c r="C11" t="n">
         <v>4.40490201882407</v>
@@ -760,13 +775,14 @@
       <c r="K11" t="n">
         <v>0</v>
       </c>
+      <c r="L11"/>
     </row>
     <row r="12">
       <c r="A12" t="n">
         <v>11</v>
       </c>
       <c r="B12" t="n">
-        <v>16</v>
+        <v>29.3370045496949</v>
       </c>
       <c r="C12" t="n">
         <v>5.1800498757296</v>
@@ -795,13 +811,14 @@
       <c r="K12" t="n">
         <v>0</v>
       </c>
+      <c r="L12"/>
     </row>
     <row r="13">
       <c r="A13" t="n">
         <v>12</v>
       </c>
       <c r="B13" t="n">
-        <v>16</v>
+        <v>25.7506826350681</v>
       </c>
       <c r="C13" t="n">
         <v>5.90148031900995</v>
@@ -830,13 +847,14 @@
       <c r="K13" t="n">
         <v>0</v>
       </c>
+      <c r="L13"/>
     </row>
     <row r="14">
       <c r="A14" t="n">
         <v>13</v>
       </c>
       <c r="B14" t="n">
-        <v>16</v>
+        <v>23.141973206503</v>
       </c>
       <c r="C14" t="n">
         <v>6.56673246554543</v>
@@ -851,7 +869,7 @@
         <v>3.60715613033392</v>
       </c>
       <c r="G14" t="n">
-        <v>5.10963369085116</v>
+        <v>6.85148511145698</v>
       </c>
       <c r="H14" t="n">
         <v>5000</v>
@@ -865,13 +883,14 @@
       <c r="K14" t="n">
         <v>1.66945381315756</v>
       </c>
+      <c r="L14"/>
     </row>
     <row r="15">
       <c r="A15" t="n">
         <v>14</v>
       </c>
       <c r="B15" t="n">
-        <v>16</v>
+        <v>21.1675331000167</v>
       </c>
       <c r="C15" t="n">
         <v>7.1792563665251</v>
@@ -886,7 +905,7 @@
         <v>3.60715613033392</v>
       </c>
       <c r="G15" t="n">
-        <v>5.10963369085116</v>
+        <v>6.85148511145698</v>
       </c>
       <c r="H15" t="n">
         <v>5000</v>
@@ -900,13 +919,14 @@
       <c r="K15" t="n">
         <v>5.25923498531434</v>
       </c>
+      <c r="L15"/>
     </row>
     <row r="16">
       <c r="A16" t="n">
         <v>15</v>
       </c>
       <c r="B16" t="n">
-        <v>16</v>
+        <v>19.5402662230243</v>
       </c>
       <c r="C16" t="n">
         <v>7.77712775442449</v>
@@ -921,7 +941,7 @@
         <v>3.60715613033392</v>
       </c>
       <c r="G16" t="n">
-        <v>5.10963369085116</v>
+        <v>6.85148511145698</v>
       </c>
       <c r="H16" t="n">
         <v>5000</v>
@@ -935,13 +955,14 @@
       <c r="K16" t="n">
         <v>4.89263932430515</v>
       </c>
+      <c r="L16"/>
     </row>
     <row r="17">
       <c r="A17" t="n">
         <v>16</v>
       </c>
       <c r="B17" t="n">
-        <v>16</v>
+        <v>18.1515298023427</v>
       </c>
       <c r="C17" t="n">
         <v>8.37213989271097</v>
@@ -956,7 +977,7 @@
         <v>3.60715613033392</v>
       </c>
       <c r="G17" t="n">
-        <v>5.10963369085116</v>
+        <v>6.85148511145698</v>
       </c>
       <c r="H17" t="n">
         <v>5000</v>
@@ -970,13 +991,14 @@
       <c r="K17" t="n">
         <v>4.5019880750606</v>
       </c>
+      <c r="L17"/>
     </row>
     <row r="18">
       <c r="A18" t="n">
         <v>17</v>
       </c>
       <c r="B18" t="n">
-        <v>16</v>
+        <v>16.9544393495548</v>
       </c>
       <c r="C18" t="n">
         <v>8.96326582311413</v>
@@ -991,7 +1013,7 @@
         <v>3.60715613033392</v>
       </c>
       <c r="G18" t="n">
-        <v>5.10963369085116</v>
+        <v>6.85148511145698</v>
       </c>
       <c r="H18" t="n">
         <v>5000</v>
@@ -1005,13 +1027,14 @@
       <c r="K18" t="n">
         <v>4.08079330164035</v>
       </c>
+      <c r="L18"/>
     </row>
     <row r="19">
       <c r="A19" t="n">
         <v>18</v>
       </c>
       <c r="B19" t="n">
-        <v>16</v>
+        <v>15.9134196230229</v>
       </c>
       <c r="C19" t="n">
         <v>9.54962229187153</v>
@@ -1026,7 +1049,7 @@
         <v>3.60715613033392</v>
       </c>
       <c r="G19" t="n">
-        <v>5.10963369085116</v>
+        <v>6.85148511145698</v>
       </c>
       <c r="H19" t="n">
         <v>5000</v>
@@ -1040,13 +1063,14 @@
       <c r="K19" t="n">
         <v>3.6062313999351</v>
       </c>
+      <c r="L19"/>
     </row>
     <row r="20">
       <c r="A20" t="n">
         <v>19</v>
       </c>
       <c r="B20" t="n">
-        <v>16</v>
+        <v>15.0010267650324</v>
       </c>
       <c r="C20" t="n">
         <v>10.1304496786956</v>
@@ -1061,7 +1085,7 @@
         <v>3.60715613033392</v>
       </c>
       <c r="G20" t="n">
-        <v>5.10963369085116</v>
+        <v>6.85148511145698</v>
       </c>
       <c r="H20" t="n">
         <v>5000</v>
@@ -1075,13 +1099,14 @@
       <c r="K20" t="n">
         <v>2.93382385143181</v>
       </c>
+      <c r="L20"/>
     </row>
     <row r="21">
       <c r="A21" t="n">
         <v>20</v>
       </c>
       <c r="B21" t="n">
-        <v>16</v>
+        <v>14.1957769489591</v>
       </c>
       <c r="C21" t="n">
         <v>10.7050954180474</v>
@@ -1096,10 +1121,10 @@
         <v>3.60715613033392</v>
       </c>
       <c r="G21" t="n">
-        <v>5.10963369085116</v>
+        <v>6.85148511145698</v>
       </c>
       <c r="H21" t="n">
-        <v>5000</v>
+        <v>3936.15889599751</v>
       </c>
       <c r="I21" t="n">
         <v>5.10963369085116</v>
@@ -1109,6 +1134,9 @@
       </c>
       <c r="K21" t="n">
         <v>2.59405230533418</v>
+      </c>
+      <c r="L21" t="n">
+        <v>1063.84110400249</v>
       </c>
     </row>
     <row r="22">
@@ -1116,7 +1144,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="n">
-        <v>16</v>
+        <v>15.1935370014656</v>
       </c>
       <c r="C22" t="n">
         <v>11.2730001541713</v>
@@ -1125,16 +1153,16 @@
         <v>11.1880669555698</v>
       </c>
       <c r="E22" t="n">
-        <v>5000</v>
+        <v>3936.15889599751</v>
       </c>
       <c r="F22" t="n">
         <v>3.60715613033392</v>
       </c>
       <c r="G22" t="n">
-        <v>5.10963369085116</v>
+        <v>6.85148511145698</v>
       </c>
       <c r="H22" t="n">
-        <v>5000</v>
+        <v>3936.15889599751</v>
       </c>
       <c r="I22" t="n">
         <v>5.10963369085116</v>
@@ -1145,13 +1173,14 @@
       <c r="K22" t="n">
         <v>2.52364782148915</v>
       </c>
+      <c r="L22"/>
     </row>
     <row r="23">
       <c r="A23" t="n">
         <v>22</v>
       </c>
       <c r="B23" t="n">
-        <v>16</v>
+        <v>14.4736596851052</v>
       </c>
       <c r="C23" t="n">
         <v>11.8336860674007</v>
@@ -1160,16 +1189,16 @@
         <v>11.7438434499932</v>
       </c>
       <c r="E23" t="n">
-        <v>5000</v>
+        <v>3936.15889599751</v>
       </c>
       <c r="F23" t="n">
         <v>3.60715613033392</v>
       </c>
       <c r="G23" t="n">
-        <v>5.10963369085116</v>
+        <v>6.85148511145698</v>
       </c>
       <c r="H23" t="n">
-        <v>5000</v>
+        <v>3936.15889599751</v>
       </c>
       <c r="I23" t="n">
         <v>5.10963369085116</v>
@@ -1180,13 +1209,14 @@
       <c r="K23" t="n">
         <v>2.45606969388842</v>
       </c>
+      <c r="L23"/>
     </row>
     <row r="24">
       <c r="A24" t="n">
         <v>23</v>
       </c>
       <c r="B24" t="n">
-        <v>16</v>
+        <v>13.8274193932111</v>
       </c>
       <c r="C24" t="n">
         <v>12.3867469474471</v>
@@ -1195,16 +1225,16 @@
         <v>12.2920255856248</v>
       </c>
       <c r="E24" t="n">
-        <v>5000</v>
+        <v>3936.15889599751</v>
       </c>
       <c r="F24" t="n">
         <v>3.60715613033392</v>
       </c>
       <c r="G24" t="n">
-        <v>5.10963369085116</v>
+        <v>6.85148511145698</v>
       </c>
       <c r="H24" t="n">
-        <v>5000</v>
+        <v>3936.15889599751</v>
       </c>
       <c r="I24" t="n">
         <v>5.10963369085116</v>
@@ -1215,13 +1245,14 @@
       <c r="K24" t="n">
         <v>2.39110347955853</v>
       </c>
+      <c r="L24"/>
     </row>
     <row r="25">
       <c r="A25" t="n">
         <v>24</v>
       </c>
       <c r="B25" t="n">
-        <v>16</v>
+        <v>13.2445768802631</v>
       </c>
       <c r="C25" t="n">
         <v>12.9318396886777</v>
@@ -1230,16 +1261,16 @@
         <v>12.8322761239352</v>
       </c>
       <c r="E25" t="n">
-        <v>5000</v>
+        <v>3936.15889599751</v>
       </c>
       <c r="F25" t="n">
         <v>3.60715613033392</v>
       </c>
       <c r="G25" t="n">
-        <v>5.10963369085116</v>
+        <v>6.85148511145698</v>
       </c>
       <c r="H25" t="n">
-        <v>5000</v>
+        <v>3936.15889599751</v>
       </c>
       <c r="I25" t="n">
         <v>5.10963369085116</v>
@@ -1250,13 +1281,14 @@
       <c r="K25" t="n">
         <v>2.32856656049331</v>
       </c>
+      <c r="L25"/>
     </row>
     <row r="26">
       <c r="A26" t="n">
         <v>25</v>
       </c>
       <c r="B26" t="n">
-        <v>16</v>
+        <v>12.7166718403304</v>
       </c>
       <c r="C26" t="n">
         <v>13.4686769549822</v>
@@ -1265,16 +1297,16 @@
         <v>13.3643129442466</v>
       </c>
       <c r="E26" t="n">
-        <v>5000</v>
+        <v>3936.15889599751</v>
       </c>
       <c r="F26" t="n">
         <v>3.60715613033392</v>
       </c>
       <c r="G26" t="n">
-        <v>5.10963369085116</v>
+        <v>6.85148511145698</v>
       </c>
       <c r="H26" t="n">
-        <v>5000</v>
+        <v>2486.58800365719</v>
       </c>
       <c r="I26" t="n">
         <v>5.10963369085116</v>
@@ -1284,6 +1316,9 @@
       </c>
       <c r="K26" t="n">
         <v>2.26830143414184</v>
+      </c>
+      <c r="L26" t="n">
+        <v>1449.57089234031</v>
       </c>
     </row>
     <row r="27">
@@ -1291,7 +1326,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="n">
-        <v>16</v>
+        <v>15.3956201078241</v>
       </c>
       <c r="C27" t="n">
         <v>13.997020815729</v>
@@ -1300,16 +1335,16 @@
         <v>13.8879027411805</v>
       </c>
       <c r="E27" t="n">
-        <v>5000</v>
+        <v>2486.58800365719</v>
       </c>
       <c r="F27" t="n">
         <v>3.60715613033392</v>
       </c>
       <c r="G27" t="n">
-        <v>5.10963369085116</v>
+        <v>6.85148511145698</v>
       </c>
       <c r="H27" t="n">
-        <v>5000</v>
+        <v>2486.58800365719</v>
       </c>
       <c r="I27" t="n">
         <v>5.10963369085116</v>
@@ -1320,13 +1355,14 @@
       <c r="K27" t="n">
         <v>2.21017069299685</v>
       </c>
+      <c r="L27"/>
     </row>
     <row r="28">
       <c r="A28" t="n">
         <v>27</v>
       </c>
       <c r="B28" t="n">
-        <v>16</v>
+        <v>14.8445000344743</v>
       </c>
       <c r="C28" t="n">
         <v>14.5166771949085</v>
@@ -1335,16 +1371,16 @@
         <v>14.4028555286282</v>
       </c>
       <c r="E28" t="n">
-        <v>5000</v>
+        <v>2486.58800365719</v>
       </c>
       <c r="F28" t="n">
         <v>3.60715613033392</v>
       </c>
       <c r="G28" t="n">
-        <v>5.10963369085116</v>
+        <v>6.85148511145698</v>
       </c>
       <c r="H28" t="n">
-        <v>5000</v>
+        <v>2486.58800365719</v>
       </c>
       <c r="I28" t="n">
         <v>5.10963369085116</v>
@@ -1355,13 +1391,14 @@
       <c r="K28" t="n">
         <v>2.15405321337887</v>
       </c>
+      <c r="L28"/>
     </row>
     <row r="29">
       <c r="A29" t="n">
         <v>28</v>
       </c>
       <c r="B29" t="n">
-        <v>16</v>
+        <v>14.3399064439011</v>
       </c>
       <c r="C29" t="n">
         <v>15.0274910065346</v>
@@ -1370,16 +1407,16 @@
         <v>14.9090198242306</v>
       </c>
       <c r="E29" t="n">
-        <v>5000</v>
+        <v>2486.58800365719</v>
       </c>
       <c r="F29" t="n">
         <v>3.60715613033392</v>
       </c>
       <c r="G29" t="n">
-        <v>5.10963369085116</v>
+        <v>6.85148511145698</v>
       </c>
       <c r="H29" t="n">
-        <v>5000</v>
+        <v>2486.58800365719</v>
       </c>
       <c r="I29" t="n">
         <v>5.10963369085116</v>
@@ -1390,13 +1427,14 @@
       <c r="K29" t="n">
         <v>2.09984122364552</v>
       </c>
+      <c r="L29"/>
     </row>
     <row r="30">
       <c r="A30" t="n">
         <v>29</v>
       </c>
       <c r="B30" t="n">
-        <v>16</v>
+        <v>13.8764937289993</v>
       </c>
       <c r="C30" t="n">
         <v>15.5293418732954</v>
@@ -1405,16 +1443,16 @@
         <v>15.4062784121127</v>
       </c>
       <c r="E30" t="n">
-        <v>5000</v>
+        <v>2486.58800365719</v>
       </c>
       <c r="F30" t="n">
         <v>3.60715613033392</v>
       </c>
       <c r="G30" t="n">
-        <v>5.10963369085116</v>
+        <v>6.85148511145698</v>
       </c>
       <c r="H30" t="n">
-        <v>5000</v>
+        <v>2486.58800365719</v>
       </c>
       <c r="I30" t="n">
         <v>5.10963369085116</v>
@@ -1425,13 +1463,14 @@
       <c r="K30" t="n">
         <v>2.04743802127097</v>
       </c>
+      <c r="L30"/>
     </row>
     <row r="31">
       <c r="A31" t="n">
         <v>30</v>
       </c>
       <c r="B31" t="n">
-        <v>16</v>
+        <v>13.4496896477077</v>
       </c>
       <c r="C31" t="n">
         <v>16.0221403441081</v>
@@ -1440,16 +1479,16 @@
         <v>15.8945446001621</v>
       </c>
       <c r="E31" t="n">
-        <v>5000</v>
+        <v>2486.58800365719</v>
       </c>
       <c r="F31" t="n">
         <v>3.60715613033392</v>
       </c>
       <c r="G31" t="n">
-        <v>5.10963369085116</v>
+        <v>6.85148511145698</v>
       </c>
       <c r="H31" t="n">
-        <v>5000</v>
+        <v>1757.16540381772</v>
       </c>
       <c r="I31" t="n">
         <v>5.10963369085116</v>
@@ -1459,6 +1498,9 @@
       </c>
       <c r="K31" t="n">
         <v>1.99675617504826</v>
+      </c>
+      <c r="L31" t="n">
+        <v>729.422599839471</v>
       </c>
     </row>
     <row r="32">
@@ -1466,7 +1508,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="n">
-        <v>16</v>
+        <v>15.5307048208743</v>
       </c>
       <c r="C32" t="n">
         <v>16.5058245409599</v>
@@ -1475,16 +1517,16 @@
         <v>16.3737589027606</v>
       </c>
       <c r="E32" t="n">
-        <v>5000</v>
+        <v>1757.16540381772</v>
       </c>
       <c r="F32" t="n">
         <v>3.60715613033392</v>
       </c>
       <c r="G32" t="n">
-        <v>5.10963369085116</v>
+        <v>6.85148511145698</v>
       </c>
       <c r="H32" t="n">
-        <v>5000</v>
+        <v>1757.16540381772</v>
       </c>
       <c r="I32" t="n">
         <v>5.10963369085116</v>
@@ -1495,13 +1537,14 @@
       <c r="K32" t="n">
         <v>1.94771609442659</v>
       </c>
+      <c r="L32"/>
     </row>
     <row r="33">
       <c r="A33" t="n">
         <v>32</v>
       </c>
       <c r="B33" t="n">
-        <v>16</v>
+        <v>15.0966841331242</v>
       </c>
       <c r="C33" t="n">
         <v>16.980357177132</v>
@@ -1510,16 +1553,16 @@
         <v>16.84388609152</v>
       </c>
       <c r="E33" t="n">
-        <v>5000</v>
+        <v>1757.16540381772</v>
       </c>
       <c r="F33" t="n">
         <v>3.60715613033392</v>
       </c>
       <c r="G33" t="n">
-        <v>5.10963369085116</v>
+        <v>6.85148511145698</v>
       </c>
       <c r="H33" t="n">
-        <v>5000</v>
+        <v>1757.16540381772</v>
       </c>
       <c r="I33" t="n">
         <v>5.10963369085116</v>
@@ -1530,13 +1573,14 @@
       <c r="K33" t="n">
         <v>1.90024487982898</v>
       </c>
+      <c r="L33"/>
     </row>
     <row r="34">
       <c r="A34" t="n">
         <v>33</v>
       </c>
       <c r="B34" t="n">
-        <v>16</v>
+        <v>14.6939791641175</v>
       </c>
       <c r="C34" t="n">
         <v>17.4457228983139</v>
@@ -1545,16 +1589,16 @@
         <v>17.3049125659091</v>
       </c>
       <c r="E34" t="n">
-        <v>5000</v>
+        <v>1757.16540381772</v>
       </c>
       <c r="F34" t="n">
         <v>3.60715613033392</v>
       </c>
       <c r="G34" t="n">
-        <v>5.10963369085116</v>
+        <v>6.85148511145698</v>
       </c>
       <c r="H34" t="n">
-        <v>5000</v>
+        <v>1757.16540381772</v>
       </c>
       <c r="I34" t="n">
         <v>5.10963369085116</v>
@@ -1565,13 +1609,14 @@
       <c r="K34" t="n">
         <v>1.8542753902673</v>
       </c>
+      <c r="L34"/>
     </row>
     <row r="35">
       <c r="A35" t="n">
         <v>34</v>
       </c>
       <c r="B35" t="n">
-        <v>16</v>
+        <v>14.3195257382184</v>
       </c>
       <c r="C35" t="n">
         <v>17.9019259057308</v>
@@ -1580,16 +1625,16 @@
         <v>17.7568440032275</v>
       </c>
       <c r="E35" t="n">
-        <v>5000</v>
+        <v>1757.16540381772</v>
       </c>
       <c r="F35" t="n">
         <v>3.60715613033392</v>
       </c>
       <c r="G35" t="n">
-        <v>5.10963369085116</v>
+        <v>6.85148511145698</v>
       </c>
       <c r="H35" t="n">
-        <v>5000</v>
+        <v>1757.16540381772</v>
       </c>
       <c r="I35" t="n">
         <v>5.10963369085116</v>
@@ -1600,13 +1645,14 @@
       <c r="K35" t="n">
         <v>1.80974548064258</v>
       </c>
+      <c r="L35"/>
     </row>
     <row r="36">
       <c r="A36" t="n">
         <v>35</v>
       </c>
       <c r="B36" t="n">
-        <v>16</v>
+        <v>13.9706392087141</v>
       </c>
       <c r="C36" t="n">
         <v>18.3489878266198</v>
@@ -1615,16 +1661,16 @@
         <v>18.1997032535443</v>
       </c>
       <c r="E36" t="n">
-        <v>5000</v>
+        <v>1757.16540381772</v>
       </c>
       <c r="F36" t="n">
         <v>3.60715613033392</v>
       </c>
       <c r="G36" t="n">
-        <v>5.10963369085116</v>
+        <v>6.85148511145698</v>
       </c>
       <c r="H36" t="n">
-        <v>5000</v>
+        <v>1339.7676344268</v>
       </c>
       <c r="I36" t="n">
         <v>5.10963369085116</v>
@@ -1634,6 +1680,9 @@
       </c>
       <c r="K36" t="n">
         <v>1.76659737275758</v>
+      </c>
+      <c r="L36" t="n">
+        <v>417.397769390921</v>
       </c>
     </row>
     <row r="37">
@@ -1641,7 +1690,7 @@
         <v>36</v>
       </c>
       <c r="B37" t="n">
-        <v>16</v>
+        <v>15.6265745494857</v>
       </c>
       <c r="C37" t="n">
         <v>18.7869458024917</v>
@@ -1650,16 +1699,16 @@
         <v>18.6335284502864</v>
       </c>
       <c r="E37" t="n">
-        <v>5000</v>
+        <v>1339.7676344268</v>
       </c>
       <c r="F37" t="n">
         <v>3.60715613033392</v>
       </c>
       <c r="G37" t="n">
-        <v>5.10963369085116</v>
+        <v>6.85148511145698</v>
       </c>
       <c r="H37" t="n">
-        <v>5000</v>
+        <v>1339.7676344268</v>
       </c>
       <c r="I37" t="n">
         <v>5.10963369085116</v>
@@ -1670,13 +1719,14 @@
       <c r="K37" t="n">
         <v>1.72477713259191</v>
       </c>
+      <c r="L37"/>
     </row>
     <row r="38">
       <c r="A38" t="n">
         <v>37</v>
       </c>
       <c r="B38" t="n">
-        <v>16</v>
+        <v>15.2777835681679</v>
       </c>
       <c r="C38" t="n">
         <v>19.2158507698372</v>
@@ -1685,16 +1735,16 @@
         <v>19.0583713113502</v>
       </c>
       <c r="E38" t="n">
-        <v>5000</v>
+        <v>1339.7676344268</v>
       </c>
       <c r="F38" t="n">
         <v>3.60715613033392</v>
       </c>
       <c r="G38" t="n">
-        <v>5.10963369085116</v>
+        <v>6.85148511145698</v>
       </c>
       <c r="H38" t="n">
-        <v>5000</v>
+        <v>1339.7676344268</v>
       </c>
       <c r="I38" t="n">
         <v>5.10963369085116</v>
@@ -1705,13 +1755,14 @@
       <c r="K38" t="n">
         <v>1.68423423270295</v>
       </c>
+      <c r="L38"/>
     </row>
     <row r="39">
       <c r="A39" t="n">
         <v>38</v>
       </c>
       <c r="B39" t="n">
-        <v>16</v>
+        <v>14.9510648305657</v>
       </c>
       <c r="C39" t="n">
         <v>19.6357659114422</v>
@@ -1720,16 +1771,16 @@
         <v>19.4742956090911</v>
       </c>
       <c r="E39" t="n">
-        <v>5000</v>
+        <v>1339.7676344268</v>
       </c>
       <c r="F39" t="n">
         <v>3.60715613033392</v>
       </c>
       <c r="G39" t="n">
-        <v>5.10963369085116</v>
+        <v>6.85148511145698</v>
       </c>
       <c r="H39" t="n">
-        <v>5000</v>
+        <v>1339.7676344268</v>
       </c>
       <c r="I39" t="n">
         <v>5.10963369085116</v>
@@ -1740,13 +1791,14 @@
       <c r="K39" t="n">
         <v>1.64492118333375</v>
       </c>
+      <c r="L39"/>
     </row>
     <row r="40">
       <c r="A40" t="n">
         <v>39</v>
       </c>
       <c r="B40" t="n">
-        <v>16</v>
+        <v>14.6445376768107</v>
       </c>
       <c r="C40" t="n">
         <v>20.0467652594219</v>
@@ -1755,16 +1807,16 @@
         <v>19.8813757904653</v>
       </c>
       <c r="E40" t="n">
-        <v>5000</v>
+        <v>1339.7676344268</v>
       </c>
       <c r="F40" t="n">
         <v>3.60715613033392</v>
       </c>
       <c r="G40" t="n">
-        <v>5.10963369085116</v>
+        <v>6.85148511145698</v>
       </c>
       <c r="H40" t="n">
-        <v>5000</v>
+        <v>1339.7676344268</v>
       </c>
       <c r="I40" t="n">
         <v>5.10963369085116</v>
@@ -1775,13 +1827,14 @@
       <c r="K40" t="n">
         <v>1.60679321937092</v>
       </c>
+      <c r="L40"/>
     </row>
     <row r="41">
       <c r="A41" t="n">
         <v>40</v>
       </c>
       <c r="B41" t="n">
-        <v>16</v>
+        <v>14.3565249723326</v>
       </c>
       <c r="C41" t="n">
         <v>20.4489324335488</v>
@@ -1790,16 +1843,16 @@
         <v>20.2796957310477</v>
       </c>
       <c r="E41" t="n">
-        <v>5000</v>
+        <v>1339.7676344268</v>
       </c>
       <c r="F41" t="n">
         <v>3.60715613033392</v>
       </c>
       <c r="G41" t="n">
-        <v>5.10963369085116</v>
+        <v>6.85148511145698</v>
       </c>
       <c r="H41" t="n">
-        <v>5000</v>
+        <v>1078.72918132365</v>
       </c>
       <c r="I41" t="n">
         <v>5.10963369085116</v>
@@ -1809,6 +1862,9 @@
       </c>
       <c r="K41" t="n">
         <v>1.56980803300933</v>
+      </c>
+      <c r="L41" t="n">
+        <v>261.038453103148</v>
       </c>
     </row>
     <row r="42">
@@ -1816,7 +1872,7 @@
         <v>41</v>
       </c>
       <c r="B42" t="n">
-        <v>16</v>
+        <v>15.6975406188226</v>
       </c>
       <c r="C42" t="n">
         <v>20.8423595005471</v>
@@ -1825,16 +1881,16 @@
         <v>20.6693476087272</v>
       </c>
       <c r="E42" t="n">
-        <v>5000</v>
+        <v>1078.72918132365</v>
       </c>
       <c r="F42" t="n">
         <v>3.60715613033392</v>
       </c>
       <c r="G42" t="n">
-        <v>5.10963369085116</v>
+        <v>6.85148511145698</v>
       </c>
       <c r="H42" t="n">
-        <v>5000</v>
+        <v>1078.72918132365</v>
       </c>
       <c r="I42" t="n">
         <v>5.10963369085116</v>
@@ -1845,13 +1901,14 @@
       <c r="K42" t="n">
         <v>1.53392554406034</v>
       </c>
+      <c r="L42"/>
     </row>
     <row r="43">
       <c r="A43" t="n">
         <v>42</v>
       </c>
       <c r="B43" t="n">
-        <v>16</v>
+        <v>15.4129898455944</v>
       </c>
       <c r="C43" t="n">
         <v>21.2271459418018</v>
@@ -1860,16 +1917,16 @@
         <v>21.0504308846446</v>
       </c>
       <c r="E43" t="n">
-        <v>5000</v>
+        <v>1078.72918132365</v>
       </c>
       <c r="F43" t="n">
         <v>3.60715613033392</v>
       </c>
       <c r="G43" t="n">
-        <v>5.10963369085116</v>
+        <v>6.85148511145698</v>
       </c>
       <c r="H43" t="n">
-        <v>5000</v>
+        <v>1078.72918132365</v>
       </c>
       <c r="I43" t="n">
         <v>5.10963369085116</v>
@@ -1880,13 +1937,14 @@
       <c r="K43" t="n">
         <v>1.49910770145416</v>
       </c>
+      <c r="L43"/>
     </row>
     <row r="44">
       <c r="A44" t="n">
         <v>43</v>
       </c>
       <c r="B44" t="n">
-        <v>16</v>
+        <v>15.1445522188633</v>
       </c>
       <c r="C44" t="n">
         <v>21.6033977184502</v>
@@ -1895,16 +1953,16 @@
         <v>21.4230513804442</v>
       </c>
       <c r="E44" t="n">
-        <v>5000</v>
+        <v>1078.72918132365</v>
       </c>
       <c r="F44" t="n">
         <v>3.60715613033392</v>
       </c>
       <c r="G44" t="n">
-        <v>5.10963369085116</v>
+        <v>6.85148511145698</v>
       </c>
       <c r="H44" t="n">
-        <v>5000</v>
+        <v>1078.72918132365</v>
       </c>
       <c r="I44" t="n">
         <v>5.10963369085116</v>
@@ -1915,13 +1973,14 @@
       <c r="K44" t="n">
         <v>1.46531831073966</v>
       </c>
+      <c r="L44"/>
     </row>
     <row r="45">
       <c r="A45" t="n">
         <v>44</v>
       </c>
       <c r="B45" t="n">
-        <v>16</v>
+        <v>14.8910114772967</v>
       </c>
       <c r="C45" t="n">
         <v>21.9712264241258</v>
@@ -1930,16 +1989,16 @@
         <v>21.7873204422018</v>
       </c>
       <c r="E45" t="n">
-        <v>5000</v>
+        <v>1078.72918132365</v>
       </c>
       <c r="F45" t="n">
         <v>3.60715613033392</v>
       </c>
       <c r="G45" t="n">
-        <v>5.10963369085116</v>
+        <v>6.85148511145698</v>
       </c>
       <c r="H45" t="n">
-        <v>5000</v>
+        <v>1078.72918132365</v>
       </c>
       <c r="I45" t="n">
         <v>5.10963369085116</v>
@@ -1950,13 +2009,14 @@
       <c r="K45" t="n">
         <v>1.43252288337442</v>
       </c>
+      <c r="L45"/>
     </row>
     <row r="46">
       <c r="A46" t="n">
         <v>45</v>
       </c>
       <c r="B46" t="n">
-        <v>16</v>
+        <v>14.6512681653531</v>
       </c>
       <c r="C46" t="n">
         <v>22.3307485167485</v>
@@ -1965,16 +2025,16 @@
         <v>22.1433541825069</v>
       </c>
       <c r="E46" t="n">
-        <v>5000</v>
+        <v>1078.72918132365</v>
       </c>
       <c r="F46" t="n">
         <v>3.60715613033392</v>
       </c>
       <c r="G46" t="n">
-        <v>5.10963369085116</v>
+        <v>6.85148511145698</v>
       </c>
       <c r="H46" t="n">
-        <v>5000</v>
+        <v>904.580342456757</v>
       </c>
       <c r="I46" t="n">
         <v>5.10963369085116</v>
@@ -1984,6 +2044,9 @@
       </c>
       <c r="K46" t="n">
         <v>1.40068850437243</v>
+      </c>
+      <c r="L46" t="n">
+        <v>174.148838866897</v>
       </c>
     </row>
     <row r="47">
@@ -1991,7 +2054,7 @@
         <v>46</v>
       </c>
       <c r="B47" t="n">
-        <v>16</v>
+        <v>15.7517268617989</v>
       </c>
       <c r="C47" t="n">
         <v>22.682084621724</v>
@@ -2000,16 +2063,16 @@
         <v>22.4912727931362</v>
       </c>
       <c r="E47" t="n">
-        <v>5000</v>
+        <v>904.580342456757</v>
       </c>
       <c r="F47" t="n">
         <v>3.60715613033392</v>
       </c>
       <c r="G47" t="n">
-        <v>5.10963369085116</v>
+        <v>6.85148511145698</v>
       </c>
       <c r="H47" t="n">
-        <v>5000</v>
+        <v>904.580342456757</v>
       </c>
       <c r="I47" t="n">
         <v>5.10963369085116</v>
@@ -2020,13 +2083,14 @@
       <c r="K47" t="n">
         <v>1.36978371549981</v>
       </c>
+      <c r="L47"/>
     </row>
     <row r="48">
       <c r="A48" t="n">
         <v>47</v>
       </c>
       <c r="B48" t="n">
-        <v>16</v>
+        <v>15.5168917528294</v>
       </c>
       <c r="C48" t="n">
         <v>23.0253588997589</v>
@@ -2035,16 +2099,16 @@
         <v>22.8311999215933</v>
       </c>
       <c r="E48" t="n">
-        <v>5000</v>
+        <v>904.580342456757</v>
       </c>
       <c r="F48" t="n">
         <v>3.60715613033392</v>
       </c>
       <c r="G48" t="n">
-        <v>5.10963369085116</v>
+        <v>6.85148511145698</v>
       </c>
       <c r="H48" t="n">
-        <v>5000</v>
+        <v>904.580342456757</v>
       </c>
       <c r="I48" t="n">
         <v>5.10963369085116</v>
@@ -2055,13 +2119,14 @@
       <c r="K48" t="n">
         <v>1.33977841170143</v>
       </c>
+      <c r="L48"/>
     </row>
     <row r="49">
       <c r="A49" t="n">
         <v>48</v>
       </c>
       <c r="B49" t="n">
-        <v>16</v>
+        <v>15.2941489325334</v>
       </c>
       <c r="C49" t="n">
         <v>23.3606984732313</v>
@@ -2070,16 +2135,16 @@
         <v>23.1632621055157</v>
       </c>
       <c r="E49" t="n">
-        <v>5000</v>
+        <v>904.580342456757</v>
       </c>
       <c r="F49" t="n">
         <v>3.60715613033392</v>
       </c>
       <c r="G49" t="n">
-        <v>5.10963369085116</v>
+        <v>6.85148511145698</v>
       </c>
       <c r="H49" t="n">
-        <v>5000</v>
+        <v>904.580342456757</v>
       </c>
       <c r="I49" t="n">
         <v>5.10963369085116</v>
@@ -2090,13 +2155,14 @@
       <c r="K49" t="n">
         <v>1.31064374884142</v>
       </c>
+      <c r="L49"/>
     </row>
     <row r="50">
       <c r="A50" t="n">
         <v>49</v>
       </c>
       <c r="B50" t="n">
-        <v>16</v>
+        <v>15.082678519749</v>
       </c>
       <c r="C50" t="n">
         <v>23.6882329056994</v>
@@ -2105,16 +2171,16 @@
         <v>23.4875882595874</v>
       </c>
       <c r="E50" t="n">
-        <v>5000</v>
+        <v>904.580342456757</v>
       </c>
       <c r="F50" t="n">
         <v>3.60715613033392</v>
       </c>
       <c r="G50" t="n">
-        <v>5.10963369085116</v>
+        <v>6.85148511145698</v>
       </c>
       <c r="H50" t="n">
-        <v>5000</v>
+        <v>904.580342456757</v>
       </c>
       <c r="I50" t="n">
         <v>5.10963369085116</v>
@@ -2125,13 +2191,14 @@
       <c r="K50" t="n">
         <v>1.28235206116132</v>
       </c>
+      <c r="L50"/>
     </row>
     <row r="51">
       <c r="A51" t="n">
         <v>50</v>
       </c>
       <c r="B51" t="n">
-        <v>16</v>
+        <v>14.881731371106</v>
       </c>
       <c r="C51" t="n">
         <v>24.0080937296916</v>
@@ -2140,16 +2207,16 @@
         <v>23.8043092101504</v>
       </c>
       <c r="E51" t="n">
-        <v>5000</v>
+        <v>904.580342456757</v>
       </c>
       <c r="F51" t="n">
         <v>3.60715613033392</v>
       </c>
       <c r="G51" t="n">
-        <v>5.10963369085116</v>
+        <v>6.85148511145698</v>
       </c>
       <c r="H51" t="n">
-        <v>5000</v>
+        <v>782.597310878223</v>
       </c>
       <c r="I51" t="n">
         <v>5.10963369085116</v>
@@ -2159,6 +2226,9 @@
       </c>
       <c r="K51" t="n">
         <v>1.25487678712236</v>
+      </c>
+      <c r="L51" t="n">
+        <v>121.983031578535</v>
       </c>
     </row>
     <row r="52">
@@ -2166,7 +2236,7 @@
         <v>51</v>
       </c>
       <c r="B52" t="n">
-        <v>15.9646528</v>
+        <v>15.7940886820793</v>
       </c>
       <c r="C52" t="n">
         <v>24.3204140184175</v>
@@ -2175,16 +2245,16 @@
         <v>24.1135572732013</v>
       </c>
       <c r="E52" t="n">
-        <v>5000</v>
+        <v>782.597310878223</v>
       </c>
       <c r="F52" t="n">
         <v>3.60715613033392</v>
       </c>
       <c r="G52" t="n">
-        <v>5.10963369085116</v>
+        <v>6.85148511145698</v>
       </c>
       <c r="H52" t="n">
-        <v>5000</v>
+        <v>782.597310878223</v>
       </c>
       <c r="I52" t="n">
         <v>5.10963369085116</v>
@@ -2195,13 +2265,14 @@
       <c r="K52" t="n">
         <v>1.22819240251256</v>
       </c>
+      <c r="L52"/>
     </row>
     <row r="53">
       <c r="A53" t="n">
         <v>52</v>
       </c>
       <c r="B53" t="n">
-        <v>15.9293056</v>
+        <v>15.5985242442717</v>
       </c>
       <c r="C53" t="n">
         <v>24.6253279974759</v>
@@ -2210,16 +2281,16 @@
         <v>24.4154658718906</v>
       </c>
       <c r="E53" t="n">
-        <v>5000</v>
+        <v>782.597310878223</v>
       </c>
       <c r="F53" t="n">
         <v>3.60715613033392</v>
       </c>
       <c r="G53" t="n">
-        <v>5.10963369085116</v>
+        <v>6.85148511145698</v>
       </c>
       <c r="H53" t="n">
-        <v>5000</v>
+        <v>782.597310878223</v>
       </c>
       <c r="I53" t="n">
         <v>5.10963369085116</v>
@@ -2230,13 +2301,14 @@
       <c r="K53" t="n">
         <v>1.20227435987322</v>
       </c>
+      <c r="L53"/>
     </row>
     <row r="54">
       <c r="A54" t="n">
         <v>53</v>
       </c>
       <c r="B54" t="n">
-        <v>15.8939584</v>
+        <v>15.4122387946049</v>
       </c>
       <c r="C54" t="n">
         <v>24.9229706930203</v>
@@ -2245,16 +2317,16 @@
         <v>24.710169190024</v>
       </c>
       <c r="E54" t="n">
-        <v>5000</v>
+        <v>782.597310878223</v>
       </c>
       <c r="F54" t="n">
         <v>3.60715613033392</v>
       </c>
       <c r="G54" t="n">
-        <v>5.10963369085116</v>
+        <v>6.85148511145698</v>
       </c>
       <c r="H54" t="n">
-        <v>5000</v>
+        <v>782.597310878223</v>
       </c>
       <c r="I54" t="n">
         <v>5.10963369085116</v>
@@ -2265,13 +2337,14 @@
       <c r="K54" t="n">
         <v>1.17709903344644</v>
       </c>
+      <c r="L54"/>
     </row>
     <row r="55">
       <c r="A55" t="n">
         <v>54</v>
       </c>
       <c r="B55" t="n">
-        <v>15.8586112</v>
+        <v>15.2346606717535</v>
       </c>
       <c r="C55" t="n">
         <v>25.2134776131879</v>
@@ -2280,16 +2353,16 @@
         <v>24.9978018584056</v>
       </c>
       <c r="E55" t="n">
-        <v>5000</v>
+        <v>782.597310878223</v>
       </c>
       <c r="F55" t="n">
         <v>3.60715613033392</v>
       </c>
       <c r="G55" t="n">
-        <v>5.10963369085116</v>
+        <v>6.85148511145698</v>
       </c>
       <c r="H55" t="n">
-        <v>5000</v>
+        <v>782.597310878223</v>
       </c>
       <c r="I55" t="n">
         <v>5.10963369085116</v>
@@ -2300,13 +2373,14 @@
       <c r="K55" t="n">
         <v>1.15264366896321</v>
       </c>
+      <c r="L55"/>
     </row>
     <row r="56">
       <c r="A56" t="n">
         <v>55</v>
       </c>
       <c r="B56" t="n">
-        <v>15.823264</v>
+        <v>15.0652629684867</v>
       </c>
       <c r="C56" t="n">
         <v>25.4969844598972</v>
@@ -2315,16 +2389,16 @@
         <v>25.2784986711622</v>
       </c>
       <c r="E56" t="n">
-        <v>5000</v>
+        <v>782.597310878223</v>
       </c>
       <c r="F56" t="n">
         <v>3.60715613033392</v>
       </c>
       <c r="G56" t="n">
-        <v>5.10963369085116</v>
+        <v>6.85148511145698</v>
       </c>
       <c r="H56" t="n">
-        <v>5000</v>
+        <v>709.453418768957</v>
       </c>
       <c r="I56" t="n">
         <v>5.10963369085116</v>
@@ -2334,6 +2408,9 @@
       </c>
       <c r="K56" t="n">
         <v>1.1288863376925</v>
+      </c>
+      <c r="L56" t="n">
+        <v>73.1438921092654</v>
       </c>
     </row>
     <row r="57">
@@ -2341,7 +2418,7 @@
         <v>56</v>
       </c>
       <c r="B57" t="n">
-        <v>15.7879168</v>
+        <v>15.6529872662952</v>
       </c>
       <c r="C57" t="n">
         <v>25.7736268683979</v>
@@ -2350,16 +2427,16 @@
         <v>25.5523943294594</v>
       </c>
       <c r="E57" t="n">
-        <v>5000</v>
+        <v>709.453418768957</v>
       </c>
       <c r="F57" t="n">
         <v>3.60715613033392</v>
       </c>
       <c r="G57" t="n">
-        <v>5.10963369085116</v>
+        <v>6.85148511145698</v>
       </c>
       <c r="H57" t="n">
-        <v>5000</v>
+        <v>709.453418768957</v>
       </c>
       <c r="I57" t="n">
         <v>5.10963369085116</v>
@@ -2370,13 +2447,14 @@
       <c r="K57" t="n">
         <v>1.1058058942546</v>
       </c>
+      <c r="L57"/>
     </row>
     <row r="58">
       <c r="A58" t="n">
         <v>57</v>
       </c>
       <c r="B58" t="n">
-        <v>15.7525696</v>
+        <v>15.490760876206</v>
       </c>
       <c r="C58" t="n">
         <v>26.043540172191</v>
@@ -2385,16 +2463,16 @@
         <v>25.8196232102565</v>
       </c>
       <c r="E58" t="n">
-        <v>5000</v>
+        <v>709.453418768957</v>
       </c>
       <c r="F58" t="n">
         <v>3.60715613033392</v>
       </c>
       <c r="G58" t="n">
-        <v>5.10963369085116</v>
+        <v>6.85148511145698</v>
       </c>
       <c r="H58" t="n">
-        <v>5000</v>
+        <v>709.453418768957</v>
       </c>
       <c r="I58" t="n">
         <v>5.10963369085116</v>
@@ -2405,13 +2483,14 @@
       <c r="K58" t="n">
         <v>1.08338193777132</v>
       </c>
+      <c r="L58"/>
     </row>
     <row r="59">
       <c r="A59" t="n">
         <v>58</v>
       </c>
       <c r="B59" t="n">
-        <v>15.7172224</v>
+        <v>15.3357058037863</v>
       </c>
       <c r="C59" t="n">
         <v>26.3068591911609</v>
@@ -2420,16 +2499,16 @@
         <v>26.0803191579658</v>
       </c>
       <c r="E59" t="n">
-        <v>5000</v>
+        <v>709.453418768957</v>
       </c>
       <c r="F59" t="n">
         <v>3.60715613033392</v>
       </c>
       <c r="G59" t="n">
-        <v>5.10963369085116</v>
+        <v>6.85148511145698</v>
       </c>
       <c r="H59" t="n">
-        <v>5000</v>
+        <v>709.453418768957</v>
       </c>
       <c r="I59" t="n">
         <v>5.10963369085116</v>
@@ -2440,13 +2519,14 @@
       <c r="K59" t="n">
         <v>1.06159477598508</v>
       </c>
+      <c r="L59"/>
     </row>
     <row r="60">
       <c r="A60" t="n">
         <v>59</v>
       </c>
       <c r="B60" t="n">
-        <v>15.6818752</v>
+        <v>15.1874166317887</v>
       </c>
       <c r="C60" t="n">
         <v>26.5637180409504</v>
@@ -2455,16 +2535,16 @@
         <v>26.3346152970701</v>
       </c>
       <c r="E60" t="n">
-        <v>5000</v>
+        <v>709.453418768957</v>
       </c>
       <c r="F60" t="n">
         <v>3.60715613033392</v>
       </c>
       <c r="G60" t="n">
-        <v>5.10963369085116</v>
+        <v>6.85148511145698</v>
       </c>
       <c r="H60" t="n">
-        <v>5000</v>
+        <v>709.453418768957</v>
       </c>
       <c r="I60" t="n">
         <v>5.10963369085116</v>
@@ -2475,13 +2555,14 @@
       <c r="K60" t="n">
         <v>1.04042539202808</v>
       </c>
+      <c r="L60"/>
     </row>
     <row r="61">
       <c r="A61" t="n">
         <v>60</v>
       </c>
       <c r="B61" t="n">
-        <v>15.646528</v>
+        <v>15.0455169826567</v>
       </c>
       <c r="C61" t="n">
         <v>26.8142499617875</v>
@@ -2490,16 +2571,16 @@
         <v>26.5826438639291</v>
       </c>
       <c r="E61" t="n">
-        <v>5000</v>
+        <v>709.453418768957</v>
       </c>
       <c r="F61" t="n">
         <v>3.60715613033392</v>
       </c>
       <c r="G61" t="n">
-        <v>5.10963369085116</v>
+        <v>6.85148511145698</v>
       </c>
       <c r="H61" t="n">
-        <v>5000</v>
+        <v>656.034081764897</v>
       </c>
       <c r="I61" t="n">
         <v>5.10963369085116</v>
@@ -2509,6 +2590,9 @@
       </c>
       <c r="K61" t="n">
         <v>1.01985541356441</v>
+      </c>
+      <c r="L61" t="n">
+        <v>53.4193370040599</v>
       </c>
     </row>
     <row r="62">
@@ -2516,7 +2600,7 @@
         <v>61</v>
       </c>
       <c r="B62" t="n">
-        <v>15.6111808</v>
+        <v>15.5048080499519</v>
       </c>
       <c r="C62" t="n">
         <v>27.0585871651294</v>
@@ -2525,16 +2609,16 @@
         <v>26.8245360561586</v>
       </c>
       <c r="E62" t="n">
-        <v>5000</v>
+        <v>656.034081764897</v>
       </c>
       <c r="F62" t="n">
         <v>3.60715613033392</v>
       </c>
       <c r="G62" t="n">
-        <v>5.10963369085116</v>
+        <v>6.85148511145698</v>
       </c>
       <c r="H62" t="n">
-        <v>5000</v>
+        <v>656.034081764897</v>
       </c>
       <c r="I62" t="n">
         <v>5.10963369085116</v>
@@ -2545,13 +2629,14 @@
       <c r="K62" t="n">
         <v>0.999867084064052</v>
       </c>
+      <c r="L62"/>
     </row>
     <row r="63">
       <c r="A63" t="n">
         <v>62</v>
       </c>
       <c r="B63" t="n">
-        <v>15.5758336</v>
+        <v>15.3694670153047</v>
       </c>
       <c r="C63" t="n">
         <v>27.2968606966301</v>
@@ -2560,16 +2645,16 @@
         <v>27.060421898107</v>
       </c>
       <c r="E63" t="n">
-        <v>5000</v>
+        <v>656.034081764897</v>
       </c>
       <c r="F63" t="n">
         <v>3.60715613033392</v>
       </c>
       <c r="G63" t="n">
-        <v>5.10963369085116</v>
+        <v>6.85148511145698</v>
       </c>
       <c r="H63" t="n">
-        <v>5000</v>
+        <v>656.034081764897</v>
       </c>
       <c r="I63" t="n">
         <v>5.10963369085116</v>
@@ -2580,13 +2665,14 @@
       <c r="K63" t="n">
         <v>0.980443235998404</v>
       </c>
+      <c r="L63"/>
     </row>
     <row r="64">
       <c r="A64" t="n">
         <v>63</v>
       </c>
       <c r="B64" t="n">
-        <v>15.5404864</v>
+        <v>15.2397525286576</v>
       </c>
       <c r="C64" t="n">
         <v>27.5292003140668</v>
@@ -2595,16 +2681,16 @@
         <v>27.2904301210825</v>
       </c>
       <c r="E64" t="n">
-        <v>5000</v>
+        <v>656.034081764897</v>
       </c>
       <c r="F64" t="n">
         <v>3.60715613033392</v>
       </c>
       <c r="G64" t="n">
-        <v>5.10963369085116</v>
+        <v>6.85148511145698</v>
       </c>
       <c r="H64" t="n">
-        <v>5000</v>
+        <v>656.034081764897</v>
       </c>
       <c r="I64" t="n">
         <v>5.10963369085116</v>
@@ -2615,13 +2701,14 @@
       <c r="K64" t="n">
         <v>0.961567265771786</v>
       </c>
+      <c r="L64"/>
     </row>
     <row r="65">
       <c r="A65" t="n">
         <v>64</v>
       </c>
       <c r="B65" t="n">
-        <v>15.5051392</v>
+        <v>15.1153701923297</v>
       </c>
       <c r="C65" t="n">
         <v>27.7557343789779</v>
@@ -2630,16 +2717,16 @@
         <v>27.5146880570955</v>
       </c>
       <c r="E65" t="n">
-        <v>5000</v>
+        <v>656.034081764897</v>
       </c>
       <c r="F65" t="n">
         <v>3.60715613033392</v>
       </c>
       <c r="G65" t="n">
-        <v>5.10963369085116</v>
+        <v>6.85148511145698</v>
       </c>
       <c r="H65" t="n">
-        <v>5000</v>
+        <v>656.034081764897</v>
       </c>
       <c r="I65" t="n">
         <v>5.10963369085116</v>
@@ -2650,13 +2737,14 @@
       <c r="K65" t="n">
         <v>0.943223110227367</v>
       </c>
+      <c r="L65"/>
     </row>
     <row r="66">
       <c r="A66" t="n">
         <v>65</v>
       </c>
       <c r="B66" t="n">
-        <v>15.469792</v>
+        <v>14.9960450392377</v>
       </c>
       <c r="C66" t="n">
         <v>27.9765897608659</v>
@@ -2665,16 +2753,16 @@
         <v>27.7333215449889</v>
       </c>
       <c r="E66" t="n">
-        <v>5000</v>
+        <v>656.034081764897</v>
       </c>
       <c r="F66" t="n">
         <v>3.60715613033392</v>
       </c>
       <c r="G66" t="n">
-        <v>5.10963369085116</v>
+        <v>6.85148511145698</v>
       </c>
       <c r="H66" t="n">
-        <v>5000</v>
+        <v>616.502971998057</v>
       </c>
       <c r="I66" t="n">
         <v>5.10963369085116</v>
@@ -2684,6 +2772,9 @@
       </c>
       <c r="K66" t="n">
         <v>0.925395224583823</v>
+      </c>
+      <c r="L66" t="n">
+        <v>39.53110976684</v>
       </c>
     </row>
     <row r="67">
@@ -2691,7 +2782,7 @@
         <v>66</v>
       </c>
       <c r="B67" t="n">
-        <v>15.4344448</v>
+        <v>15.3512203384628</v>
       </c>
       <c r="C67" t="n">
         <v>28.1918917529209</v>
@@ -2700,16 +2791,16 @@
         <v>27.9464548479187</v>
       </c>
       <c r="E67" t="n">
-        <v>5000</v>
+        <v>616.502971998057</v>
       </c>
       <c r="F67" t="n">
         <v>3.60715613033392</v>
       </c>
       <c r="G67" t="n">
-        <v>5.10963369085116</v>
+        <v>6.85148511145698</v>
       </c>
       <c r="H67" t="n">
-        <v>5000</v>
+        <v>616.502971998057</v>
       </c>
       <c r="I67" t="n">
         <v>5.10963369085116</v>
@@ -2720,13 +2811,14 @@
       <c r="K67" t="n">
         <v>0.908068561676281</v>
       </c>
+      <c r="L67"/>
     </row>
     <row r="68">
       <c r="A68" t="n">
         <v>67</v>
       </c>
       <c r="B68" t="n">
-        <v>15.3990976</v>
+        <v>15.2377838955039</v>
       </c>
       <c r="C68" t="n">
         <v>28.401763998299</v>
@@ -2735,16 +2827,16 @@
         <v>28.1542105812381</v>
       </c>
       <c r="E68" t="n">
-        <v>5000</v>
+        <v>616.502971998057</v>
       </c>
       <c r="F68" t="n">
         <v>3.60715613033392</v>
       </c>
       <c r="G68" t="n">
-        <v>5.10963369085116</v>
+        <v>6.85148511145698</v>
       </c>
       <c r="H68" t="n">
-        <v>5000</v>
+        <v>616.502971998057</v>
       </c>
       <c r="I68" t="n">
         <v>5.10963369085116</v>
@@ -2755,13 +2847,14 @@
       <c r="K68" t="n">
         <v>0.89122855238936</v>
       </c>
+      <c r="L68"/>
     </row>
     <row r="69">
       <c r="A69" t="n">
         <v>68</v>
       </c>
       <c r="B69" t="n">
-        <v>15.3637504</v>
+        <v>15.1288181975382</v>
       </c>
       <c r="C69" t="n">
         <v>28.6063284260766</v>
@@ -2770,16 +2863,16 @@
         <v>28.3567096499117</v>
       </c>
       <c r="E69" t="n">
-        <v>5000</v>
+        <v>616.502971998057</v>
       </c>
       <c r="F69" t="n">
         <v>3.60715613033392</v>
       </c>
       <c r="G69" t="n">
-        <v>5.10963369085116</v>
+        <v>6.85148511145698</v>
       </c>
       <c r="H69" t="n">
-        <v>5000</v>
+        <v>616.502971998057</v>
       </c>
       <c r="I69" t="n">
         <v>5.10963369085116</v>
@@ -2790,13 +2883,14 @@
       <c r="K69" t="n">
         <v>0.87486108718233</v>
       </c>
+      <c r="L69"/>
     </row>
     <row r="70">
       <c r="A70" t="n">
         <v>69</v>
       </c>
       <c r="B70" t="n">
-        <v>15.3284032</v>
+        <v>15.0241050899972</v>
       </c>
       <c r="C70" t="n">
         <v>28.8057051960666</v>
@@ -2805,16 +2899,16 @@
         <v>28.5540711946603</v>
       </c>
       <c r="E70" t="n">
-        <v>5000</v>
+        <v>616.502971998057</v>
       </c>
       <c r="F70" t="n">
         <v>3.60715613033392</v>
       </c>
       <c r="G70" t="n">
-        <v>5.10963369085116</v>
+        <v>6.85148511145698</v>
       </c>
       <c r="H70" t="n">
-        <v>5000</v>
+        <v>616.502971998057</v>
       </c>
       <c r="I70" t="n">
         <v>5.10963369085116</v>
@@ -2825,13 +2919,14 @@
       <c r="K70" t="n">
         <v>0.85895249861807</v>
       </c>
+      <c r="L70"/>
     </row>
     <row r="71">
       <c r="A71" t="n">
         <v>70</v>
       </c>
       <c r="B71" t="n">
-        <v>15.293056</v>
+        <v>14.923439767224</v>
       </c>
       <c r="C71" t="n">
         <v>29.0000126517539</v>
@@ -2840,16 +2935,16 @@
         <v>28.7464125461002</v>
       </c>
       <c r="E71" t="n">
-        <v>5000</v>
+        <v>616.502971998057</v>
       </c>
       <c r="F71" t="n">
         <v>3.60715613033392</v>
       </c>
       <c r="G71" t="n">
-        <v>5.10963369085116</v>
+        <v>6.85148511145698</v>
       </c>
       <c r="H71" t="n">
-        <v>5000</v>
+        <v>587.095484437059</v>
       </c>
       <c r="I71" t="n">
         <v>5.10963369085116</v>
@@ -2859,6 +2954,9 @@
       </c>
       <c r="K71" t="n">
         <v>0.843489544815062</v>
+      </c>
+      <c r="L71" t="n">
+        <v>29.407487560998</v>
       </c>
     </row>
     <row r="72">
@@ -2866,7 +2964,7 @@
         <v>71</v>
       </c>
       <c r="B72" t="n">
-        <v>15.2577088</v>
+        <v>15.1934240952043</v>
       </c>
       <c r="C72" t="n">
         <v>29.1893672806629</v>
@@ -2875,16 +2973,16 @@
         <v>28.9338491862015</v>
       </c>
       <c r="E72" t="n">
-        <v>5000</v>
+        <v>587.095484437059</v>
       </c>
       <c r="F72" t="n">
         <v>3.60715613033392</v>
       </c>
       <c r="G72" t="n">
-        <v>5.10963369085116</v>
+        <v>6.85148511145698</v>
       </c>
       <c r="H72" t="n">
-        <v>5000</v>
+        <v>587.095484437059</v>
       </c>
       <c r="I72" t="n">
         <v>5.10963369085116</v>
@@ -2895,13 +2993,14 @@
       <c r="K72" t="n">
         <v>0.828459393753121</v>
       </c>
+      <c r="L72"/>
     </row>
     <row r="73">
       <c r="A73" t="n">
         <v>72</v>
       </c>
       <c r="B73" t="n">
-        <v>15.2223616</v>
+        <v>15.0979843514766</v>
       </c>
       <c r="C73" t="n">
         <v>29.3738836815273</v>
@@ -2910,16 +3009,16 @@
         <v>29.116494716442</v>
       </c>
       <c r="E73" t="n">
-        <v>5000</v>
+        <v>587.095484437059</v>
       </c>
       <c r="F73" t="n">
         <v>3.60715613033392</v>
       </c>
       <c r="G73" t="n">
-        <v>5.10963369085116</v>
+        <v>6.85148511145698</v>
       </c>
       <c r="H73" t="n">
-        <v>5000</v>
+        <v>587.095484437059</v>
       </c>
       <c r="I73" t="n">
         <v>5.10963369085116</v>
@@ -2930,13 +3029,14 @@
       <c r="K73" t="n">
         <v>0.813849608366953</v>
       </c>
+      <c r="L73"/>
     </row>
     <row r="74">
       <c r="A74" t="n">
         <v>73</v>
       </c>
       <c r="B74" t="n">
-        <v>15.1870144</v>
+        <v>15.006135213418</v>
       </c>
       <c r="C74" t="n">
         <v>29.5536745376812</v>
@@ -2945,16 +3045,16 @@
         <v>29.2944608320842</v>
       </c>
       <c r="E74" t="n">
-        <v>5000</v>
+        <v>587.095484437059</v>
       </c>
       <c r="F74" t="n">
         <v>3.60715613033392</v>
       </c>
       <c r="G74" t="n">
-        <v>5.10963369085116</v>
+        <v>6.85148511145698</v>
       </c>
       <c r="H74" t="n">
-        <v>5000</v>
+        <v>587.095484437059</v>
       </c>
       <c r="I74" t="n">
         <v>5.10963369085116</v>
@@ -2965,13 +3065,14 @@
       <c r="K74" t="n">
         <v>0.799648132371279</v>
       </c>
+      <c r="L74"/>
     </row>
     <row r="75">
       <c r="A75" t="n">
         <v>74</v>
       </c>
       <c r="B75" t="n">
-        <v>15.1516672</v>
+        <v>14.9177121642039</v>
       </c>
       <c r="C75" t="n">
         <v>29.728850596137</v>
@@ -2980,16 +3081,16 @@
         <v>29.4678573020492</v>
       </c>
       <c r="E75" t="n">
-        <v>5000</v>
+        <v>587.095484437059</v>
       </c>
       <c r="F75" t="n">
         <v>3.60715613033392</v>
       </c>
       <c r="G75" t="n">
-        <v>5.10963369085116</v>
+        <v>6.85148511145698</v>
       </c>
       <c r="H75" t="n">
-        <v>5000</v>
+        <v>587.095484437059</v>
       </c>
       <c r="I75" t="n">
         <v>5.10963369085116</v>
@@ -3000,13 +3101,14 @@
       <c r="K75" t="n">
         <v>0.785843276765254</v>
       </c>
+      <c r="L75"/>
     </row>
     <row r="76">
       <c r="A76" t="n">
         <v>75</v>
       </c>
       <c r="B76" t="n">
-        <v>15.11632</v>
+        <v>14.8325600711007</v>
       </c>
       <c r="C76" t="n">
         <v>29.8995206518575</v>
@@ -3015,16 +3117,16 @@
         <v>29.6367919538989</v>
       </c>
       <c r="E76" t="n">
-        <v>5000</v>
+        <v>587.095484437059</v>
       </c>
       <c r="F76" t="n">
         <v>3.60715613033392</v>
       </c>
       <c r="G76" t="n">
-        <v>5.10963369085116</v>
+        <v>6.85148511145698</v>
       </c>
       <c r="H76" t="n">
-        <v>5000</v>
+        <v>565.292296150542</v>
       </c>
       <c r="I76" t="n">
         <v>5.10963369085116</v>
@@ -3034,6 +3136,9 @@
       </c>
       <c r="K76" t="n">
         <v>0.772423706968922</v>
+      </c>
+      <c r="L76" t="n">
+        <v>21.8031882865179</v>
       </c>
     </row>
     <row r="77">
@@ -3041,7 +3146,7 @@
         <v>76</v>
       </c>
       <c r="B77" t="n">
-        <v>15.0809728</v>
+        <v>15.032303527946</v>
       </c>
       <c r="C77" t="n">
         <v>30.0657915367683</v>
@@ -3050,16 +3155,16 @@
         <v>29.8013706634817</v>
       </c>
       <c r="E77" t="n">
-        <v>5000</v>
+        <v>565.292296150542</v>
       </c>
       <c r="F77" t="n">
         <v>3.60715613033392</v>
       </c>
       <c r="G77" t="n">
-        <v>5.10963369085116</v>
+        <v>6.85148511145698</v>
       </c>
       <c r="H77" t="n">
-        <v>5000</v>
+        <v>565.292296150542</v>
       </c>
       <c r="I77" t="n">
         <v>5.10963369085116</v>
@@ -3070,13 +3175,14 @@
       <c r="K77" t="n">
         <v>0.75937843054923</v>
       </c>
+      <c r="L77"/>
     </row>
     <row r="78">
       <c r="A78" t="n">
         <v>77</v>
       </c>
       <c r="B78" t="n">
-        <v>15.0456256</v>
+        <v>14.9517523919641</v>
       </c>
       <c r="C78" t="n">
         <v>30.2277681130913</v>
@@ -3085,16 +3191,16 @@
         <v>29.9616973488266</v>
       </c>
       <c r="E78" t="n">
-        <v>5000</v>
+        <v>565.292296150542</v>
       </c>
       <c r="F78" t="n">
         <v>3.60715613033392</v>
       </c>
       <c r="G78" t="n">
-        <v>5.10963369085116</v>
+        <v>6.85148511145698</v>
       </c>
       <c r="H78" t="n">
-        <v>5000</v>
+        <v>565.292296150542</v>
       </c>
       <c r="I78" t="n">
         <v>5.10963369085116</v>
@@ -3105,13 +3211,14 @@
       <c r="K78" t="n">
         <v>0.746696785497291</v>
       </c>
+      <c r="L78"/>
     </row>
     <row r="79">
       <c r="A79" t="n">
         <v>78</v>
       </c>
       <c r="B79" t="n">
-        <v>15.0102784</v>
+        <v>14.8741113964094</v>
       </c>
       <c r="C79" t="n">
         <v>30.3855532706144</v>
@@ -3120,16 +3227,16 @@
         <v>30.1178739679064</v>
       </c>
       <c r="E79" t="n">
-        <v>5000</v>
+        <v>565.292296150542</v>
       </c>
       <c r="F79" t="n">
         <v>3.60715613033392</v>
       </c>
       <c r="G79" t="n">
-        <v>5.10963369085116</v>
+        <v>6.85148511145698</v>
       </c>
       <c r="H79" t="n">
-        <v>5000</v>
+        <v>565.292296150542</v>
       </c>
       <c r="I79" t="n">
         <v>5.10963369085116</v>
@@ -3140,13 +3247,14 @@
       <c r="K79" t="n">
         <v>0.734368429020803</v>
       </c>
+      <c r="L79"/>
     </row>
     <row r="80">
       <c r="A80" t="n">
         <v>79</v>
       </c>
       <c r="B80" t="n">
-        <v>14.9749312</v>
+        <v>14.7992545612453</v>
       </c>
       <c r="C80" t="n">
         <v>30.5392479275401</v>
@@ -3155,16 +3263,16 @@
         <v>30.2700005199189</v>
       </c>
       <c r="E80" t="n">
-        <v>5000</v>
+        <v>565.292296150542</v>
       </c>
       <c r="F80" t="n">
         <v>3.60715613033392</v>
       </c>
       <c r="G80" t="n">
-        <v>5.10963369085116</v>
+        <v>6.85148511145698</v>
       </c>
       <c r="H80" t="n">
-        <v>5000</v>
+        <v>565.292296150542</v>
       </c>
       <c r="I80" t="n">
         <v>5.10963369085116</v>
@@ -3175,13 +3283,14 @@
       <c r="K80" t="n">
         <v>0.722383326820496</v>
       </c>
+      <c r="L80"/>
     </row>
     <row r="81">
       <c r="A81" t="n">
         <v>80</v>
       </c>
       <c r="B81" t="n">
-        <v>14.939584</v>
+        <v>14.7270626382537</v>
       </c>
       <c r="C81" t="n">
         <v>30.6889510345862</v>
@@ -3190,16 +3299,16 @@
         <v>30.4181750497618</v>
       </c>
       <c r="E81" t="n">
-        <v>5000</v>
+        <v>565.292296150542</v>
       </c>
       <c r="F81" t="n">
         <v>3.60715613033392</v>
       </c>
       <c r="G81" t="n">
-        <v>5.10963369085116</v>
+        <v>6.85148511145698</v>
       </c>
       <c r="H81" t="n">
-        <v>5000</v>
+        <v>549.354359055555</v>
       </c>
       <c r="I81" t="n">
         <v>5.10963369085116</v>
@@ -3209,6 +3318,9 @@
       </c>
       <c r="K81" t="n">
         <v>0.71073174282037</v>
+      </c>
+      <c r="L81" t="n">
+        <v>15.9379370949866</v>
       </c>
     </row>
     <row r="82">
@@ -3216,7 +3328,7 @@
         <v>81</v>
       </c>
       <c r="B82" t="n">
-        <v>14.9042368</v>
+        <v>14.8685239810456</v>
       </c>
       <c r="C82" t="n">
         <v>30.8347595820338</v>
@@ -3225,16 +3337,16 @@
         <v>30.5624936554035</v>
       </c>
       <c r="E82" t="n">
-        <v>5000</v>
+        <v>549.354359055555</v>
       </c>
       <c r="F82" t="n">
         <v>3.60715613033392</v>
       </c>
       <c r="G82" t="n">
-        <v>5.10963369085116</v>
+        <v>6.85148511145698</v>
       </c>
       <c r="H82" t="n">
-        <v>5000</v>
+        <v>549.354359055555</v>
       </c>
       <c r="I82" t="n">
         <v>5.10963369085116</v>
@@ -3245,13 +3357,14 @@
       <c r="K82" t="n">
         <v>0.699404229324742</v>
       </c>
+      <c r="L82"/>
     </row>
     <row r="83">
       <c r="A83" t="n">
         <v>82</v>
       </c>
       <c r="B83" t="n">
-        <v>14.8688896</v>
+        <v>14.8003611375867</v>
       </c>
       <c r="C83" t="n">
         <v>30.9767686094452</v>
@@ -3260,16 +3373,16 @@
         <v>30.703050497873</v>
       </c>
       <c r="E83" t="n">
-        <v>5000</v>
+        <v>549.354359055555</v>
       </c>
       <c r="F83" t="n">
         <v>3.60715613033392</v>
       </c>
       <c r="G83" t="n">
-        <v>5.10963369085116</v>
+        <v>6.85148511145698</v>
       </c>
       <c r="H83" t="n">
-        <v>5000</v>
+        <v>549.354359055555</v>
       </c>
       <c r="I83" t="n">
         <v>5.10963369085116</v>
@@ -3280,13 +3393,14 @@
       <c r="K83" t="n">
         <v>0.688391617578576</v>
       </c>
+      <c r="L83"/>
     </row>
     <row r="84">
       <c r="A84" t="n">
         <v>83</v>
       </c>
       <c r="B84" t="n">
-        <v>14.8335424</v>
+        <v>14.7345753794419</v>
       </c>
       <c r="C84" t="n">
         <v>31.1150712177911</v>
@@ -3295,16 +3409,16 @@
         <v>30.8399378136168</v>
       </c>
       <c r="E84" t="n">
-        <v>5000</v>
+        <v>549.354359055555</v>
       </c>
       <c r="F84" t="n">
         <v>3.60715613033392</v>
       </c>
       <c r="G84" t="n">
-        <v>5.10963369085116</v>
+        <v>6.85148511145698</v>
       </c>
       <c r="H84" t="n">
-        <v>5000</v>
+        <v>549.354359055555</v>
       </c>
       <c r="I84" t="n">
         <v>5.10963369085116</v>
@@ -3315,13 +3429,14 @@
       <c r="K84" t="n">
         <v>0.677685008706421</v>
       </c>
+      <c r="L84"/>
     </row>
     <row r="85">
       <c r="A85" t="n">
         <v>84</v>
       </c>
       <c r="B85" t="n">
-        <v>14.7981952</v>
+        <v>14.671068932149</v>
       </c>
       <c r="C85" t="n">
         <v>31.2497585837523</v>
@@ -3330,16 +3445,16 @@
         <v>30.9732459289862</v>
       </c>
       <c r="E85" t="n">
-        <v>5000</v>
+        <v>549.354359055555</v>
       </c>
       <c r="F85" t="n">
         <v>3.60715613033392</v>
       </c>
       <c r="G85" t="n">
-        <v>5.10963369085116</v>
+        <v>6.85148511145698</v>
       </c>
       <c r="H85" t="n">
-        <v>5000</v>
+        <v>549.354359055555</v>
       </c>
       <c r="I85" t="n">
         <v>5.10963369085116</v>
@@ -3350,13 +3465,14 @@
       <c r="K85" t="n">
         <v>0.667275765010471</v>
       </c>
+      <c r="L85"/>
     </row>
     <row r="86">
       <c r="A86" t="n">
         <v>85</v>
       </c>
       <c r="B86" t="n">
-        <v>14.762848</v>
+        <v>14.6097489380896</v>
       </c>
       <c r="C86" t="n">
         <v>31.380919975973</v>
@@ -3365,16 +3481,16 @@
         <v>31.1030632766398</v>
       </c>
       <c r="E86" t="n">
-        <v>5000</v>
+        <v>549.354359055555</v>
       </c>
       <c r="F86" t="n">
         <v>3.60715613033392</v>
       </c>
       <c r="G86" t="n">
-        <v>5.10963369085116</v>
+        <v>6.85148511145698</v>
       </c>
       <c r="H86" t="n">
-        <v>5000</v>
+        <v>538.049253542752</v>
       </c>
       <c r="I86" t="n">
         <v>5.10963369085116</v>
@@ -3384,6 +3500,9 @@
       </c>
       <c r="K86" t="n">
         <v>0.657155501608081</v>
+      </c>
+      <c r="L86" t="n">
+        <v>11.3051055128027</v>
       </c>
     </row>
     <row r="87">
@@ -3391,7 +3510,7 @@
         <v>86</v>
       </c>
       <c r="B87" t="n">
-        <v>14.7275008</v>
+        <v>14.7025951487525</v>
       </c>
       <c r="C87" t="n">
         <v>31.5086427730657</v>
@@ -3400,16 +3519,16 @@
         <v>31.2294764136614</v>
       </c>
       <c r="E87" t="n">
-        <v>5000</v>
+        <v>538.049253542752</v>
       </c>
       <c r="F87" t="n">
         <v>3.60715613033392</v>
       </c>
       <c r="G87" t="n">
-        <v>5.10963369085116</v>
+        <v>6.85148511145698</v>
       </c>
       <c r="H87" t="n">
-        <v>5000</v>
+        <v>538.049253542752</v>
       </c>
       <c r="I87" t="n">
         <v>5.10963369085116</v>
@@ -3420,13 +3539,14 @@
       <c r="K87" t="n">
         <v>0.647316078389917</v>
       </c>
+      <c r="L87"/>
     </row>
     <row r="88">
       <c r="A88" t="n">
         <v>87</v>
       </c>
       <c r="B88" t="n">
-        <v>14.6921536</v>
+        <v>14.6447897943764</v>
       </c>
       <c r="C88" t="n">
         <v>31.6330124831797</v>
@@ -3435,16 +3555,16 @@
         <v>31.3525700412095</v>
       </c>
       <c r="E88" t="n">
-        <v>5000</v>
+        <v>538.049253542752</v>
       </c>
       <c r="F88" t="n">
         <v>3.60715613033392</v>
       </c>
       <c r="G88" t="n">
-        <v>5.10963369085116</v>
+        <v>6.85148511145698</v>
       </c>
       <c r="H88" t="n">
-        <v>5000</v>
+        <v>538.049253542752</v>
       </c>
       <c r="I88" t="n">
         <v>5.10963369085116</v>
@@ -3455,13 +3575,14 @@
       <c r="K88" t="n">
         <v>0.637749592283608</v>
       </c>
+      <c r="L88"/>
     </row>
     <row r="89">
       <c r="A89" t="n">
         <v>88</v>
       </c>
       <c r="B89" t="n">
-        <v>14.6568064</v>
+        <v>14.5889391339014</v>
       </c>
       <c r="C89" t="n">
         <v>31.7541127649605</v>
@@ -3470,16 +3591,16 @@
         <v>31.4724270255283</v>
       </c>
       <c r="E89" t="n">
-        <v>5000</v>
+        <v>538.049253542752</v>
       </c>
       <c r="F89" t="n">
         <v>3.60715613033392</v>
       </c>
       <c r="G89" t="n">
-        <v>5.10963369085116</v>
+        <v>6.85148511145698</v>
       </c>
       <c r="H89" t="n">
-        <v>5000</v>
+        <v>538.049253542752</v>
       </c>
       <c r="I89" t="n">
         <v>5.10963369085116</v>
@@ -3490,13 +3611,14 @@
       <c r="K89" t="n">
         <v>0.628448369805976</v>
       </c>
+      <c r="L89"/>
     </row>
     <row r="90">
       <c r="A90" t="n">
         <v>89</v>
       </c>
       <c r="B90" t="n">
-        <v>14.6214592</v>
+        <v>14.5349663801426</v>
       </c>
       <c r="C90" t="n">
         <v>31.8720254497422</v>
@@ -3505,16 +3627,16 @@
         <v>31.5891284201634</v>
       </c>
       <c r="E90" t="n">
-        <v>5000</v>
+        <v>538.049253542752</v>
       </c>
       <c r="F90" t="n">
         <v>3.60715613033392</v>
       </c>
       <c r="G90" t="n">
-        <v>5.10963369085116</v>
+        <v>6.85148511145698</v>
       </c>
       <c r="H90" t="n">
-        <v>5000</v>
+        <v>538.049253542752</v>
       </c>
       <c r="I90" t="n">
         <v>5.10963369085116</v>
@@ -3525,13 +3647,14 @@
       <c r="K90" t="n">
         <v>0.619404959890621</v>
       </c>
+      <c r="L90"/>
     </row>
     <row r="91">
       <c r="A91" t="n">
         <v>90</v>
       </c>
       <c r="B91" t="n">
-        <v>14.586112</v>
+        <v>14.4827983954271</v>
       </c>
       <c r="C91" t="n">
         <v>31.9868305648254</v>
@@ -3540,16 +3663,16 @@
         <v>31.7027534892392</v>
       </c>
       <c r="E91" t="n">
-        <v>5000</v>
+        <v>538.049253542752</v>
       </c>
       <c r="F91" t="n">
         <v>3.60715613033392</v>
       </c>
       <c r="G91" t="n">
-        <v>5.10963369085116</v>
+        <v>6.85148511145698</v>
       </c>
       <c r="H91" t="n">
-        <v>5000</v>
+        <v>530.483847465811</v>
       </c>
       <c r="I91" t="n">
         <v>5.10963369085116</v>
@@ -3559,6 +3682,9 @@
       </c>
       <c r="K91" t="n">
         <v>0.610612126977259</v>
+      </c>
+      <c r="L91" t="n">
+        <v>7.56540607694149</v>
       </c>
     </row>
     <row r="92">
@@ -3566,7 +3692,7 @@
         <v>91</v>
       </c>
       <c r="B92" t="n">
-        <v>14.5507648</v>
+        <v>14.5349135324191</v>
       </c>
       <c r="C92" t="n">
         <v>32.0986063577063</v>
@@ -3575,16 +3701,16 @@
         <v>31.8133797316641</v>
       </c>
       <c r="E92" t="n">
-        <v>5000</v>
+        <v>530.483847465811</v>
       </c>
       <c r="F92" t="n">
         <v>3.60715613033392</v>
       </c>
       <c r="G92" t="n">
-        <v>5.10963369085116</v>
+        <v>6.85148511145698</v>
       </c>
       <c r="H92" t="n">
-        <v>5000</v>
+        <v>530.483847465811</v>
       </c>
       <c r="I92" t="n">
         <v>5.10963369085116</v>
@@ -3595,13 +3721,14 @@
       <c r="K92" t="n">
         <v>0.602062844349278</v>
       </c>
+      <c r="L92"/>
     </row>
     <row r="93">
       <c r="A93" t="n">
         <v>92</v>
       </c>
       <c r="B93" t="n">
-        <v>14.5154176</v>
+        <v>14.4858027403726</v>
       </c>
       <c r="C93" t="n">
         <v>32.2074293211325</v>
@@ -3610,16 +3737,16 @@
         <v>31.921082906141</v>
       </c>
       <c r="E93" t="n">
-        <v>5000</v>
+        <v>530.483847465811</v>
       </c>
       <c r="F93" t="n">
         <v>3.60715613033392</v>
       </c>
       <c r="G93" t="n">
-        <v>5.10963369085116</v>
+        <v>6.85148511145698</v>
       </c>
       <c r="H93" t="n">
-        <v>5000</v>
+        <v>530.483847465811</v>
       </c>
       <c r="I93" t="n">
         <v>5.10963369085116</v>
@@ -3630,13 +3757,14 @@
       <c r="K93" t="n">
         <v>0.59375028771007</v>
       </c>
+      <c r="L93"/>
     </row>
     <row r="94">
       <c r="A94" t="n">
         <v>93</v>
       </c>
       <c r="B94" t="n">
-        <v>14.4800704</v>
+        <v>14.4383085703245</v>
       </c>
       <c r="C94" t="n">
         <v>32.3133742188704</v>
@@ -3645,16 +3773,16 @@
         <v>32.0259370568715</v>
       </c>
       <c r="E94" t="n">
-        <v>5000</v>
+        <v>530.483847465811</v>
       </c>
       <c r="F94" t="n">
         <v>3.60715613033392</v>
       </c>
       <c r="G94" t="n">
-        <v>5.10963369085116</v>
+        <v>6.85148511145698</v>
       </c>
       <c r="H94" t="n">
-        <v>5000</v>
+        <v>530.483847465811</v>
       </c>
       <c r="I94" t="n">
         <v>5.10963369085116</v>
@@ -3665,13 +3793,14 @@
       <c r="K94" t="n">
         <v>0.585667828984965</v>
       </c>
+      <c r="L94"/>
     </row>
     <row r="95">
       <c r="A95" t="n">
         <v>94</v>
       </c>
       <c r="B95" t="n">
-        <v>14.4447232</v>
+        <v>14.3923700835731</v>
       </c>
       <c r="C95" t="n">
         <v>32.4165141120796</v>
@@ -3680,16 +3809,16 @@
         <v>32.1280145398487</v>
       </c>
       <c r="E95" t="n">
-        <v>5000</v>
+        <v>530.483847465811</v>
       </c>
       <c r="F95" t="n">
         <v>3.60715613033392</v>
       </c>
       <c r="G95" t="n">
-        <v>5.10963369085116</v>
+        <v>6.85148511145698</v>
       </c>
       <c r="H95" t="n">
-        <v>5000</v>
+        <v>530.483847465811</v>
       </c>
       <c r="I95" t="n">
         <v>5.10963369085116</v>
@@ -3700,13 +3829,14 @@
       <c r="K95" t="n">
         <v>0.57780903033968</v>
       </c>
+      <c r="L95"/>
     </row>
     <row r="96">
       <c r="A96" t="n">
         <v>95</v>
       </c>
       <c r="B96" t="n">
-        <v>14.409376</v>
+        <v>14.3479290898179</v>
       </c>
       <c r="C96" t="n">
         <v>32.5169203861976</v>
@@ -3715,16 +3845,16 @@
         <v>32.2273860496452</v>
       </c>
       <c r="E96" t="n">
-        <v>5000</v>
+        <v>530.483847465811</v>
       </c>
       <c r="F96" t="n">
         <v>3.60715613033392</v>
       </c>
       <c r="G96" t="n">
-        <v>5.10963369085116</v>
+        <v>6.85148511145698</v>
       </c>
       <c r="H96" t="n">
-        <v>5000</v>
+        <v>525.998504041046</v>
       </c>
       <c r="I96" t="n">
         <v>5.10963369085116</v>
@@ -3734,6 +3864,9 @@
       </c>
       <c r="K96" t="n">
         <v>0.570167638406236</v>
+      </c>
+      <c r="L96" t="n">
+        <v>4.48534342476489</v>
       </c>
     </row>
     <row r="97">
@@ -3741,7 +3874,7 @@
         <v>96</v>
       </c>
       <c r="B97" t="n">
-        <v>14.3740288</v>
+        <v>14.365791691678</v>
       </c>
       <c r="C97" t="n">
         <v>32.6146627782442</v>
@@ -3750,16 +3883,16 @@
         <v>32.3241206466063</v>
       </c>
       <c r="E97" t="n">
-        <v>5000</v>
+        <v>525.998504041046</v>
       </c>
       <c r="F97" t="n">
         <v>3.60715613033392</v>
       </c>
       <c r="G97" t="n">
-        <v>5.10963369085116</v>
+        <v>6.85148511145698</v>
       </c>
       <c r="H97" t="n">
-        <v>5000</v>
+        <v>525.998504041046</v>
       </c>
       <c r="I97" t="n">
         <v>5.10963369085116</v>
@@ -3770,13 +3903,14 @@
       <c r="K97" t="n">
         <v>0.562737578705718</v>
       </c>
+      <c r="L97"/>
     </row>
     <row r="98">
       <c r="A98" t="n">
         <v>97</v>
       </c>
       <c r="B98" t="n">
-        <v>14.3386816</v>
+        <v>14.3240043307195</v>
       </c>
       <c r="C98" t="n">
         <v>32.7098094044659</v>
@@ -3785,16 +3919,16 @@
         <v>32.4182857843702</v>
       </c>
       <c r="E98" t="n">
-        <v>5000</v>
+        <v>525.998504041046</v>
       </c>
       <c r="F98" t="n">
         <v>3.60715613033392</v>
       </c>
       <c r="G98" t="n">
-        <v>5.10963369085116</v>
+        <v>6.85148511145698</v>
       </c>
       <c r="H98" t="n">
-        <v>5000</v>
+        <v>525.998504041046</v>
       </c>
       <c r="I98" t="n">
         <v>5.10963369085116</v>
@@ -3805,13 +3939,14 @@
       <c r="K98" t="n">
         <v>0.555512950260969</v>
       </c>
+      <c r="L98"/>
     </row>
     <row r="99">
       <c r="A99" t="n">
         <v>98</v>
       </c>
       <c r="B99" t="n">
-        <v>14.3033344</v>
+        <v>14.2835606216338</v>
       </c>
       <c r="C99" t="n">
         <v>32.8024267882435</v>
@@ -3820,16 +3955,16 @@
         <v>32.50994733764</v>
       </c>
       <c r="E99" t="n">
-        <v>5000</v>
+        <v>525.998504041046</v>
       </c>
       <c r="F99" t="n">
         <v>3.60715613033392</v>
       </c>
       <c r="G99" t="n">
-        <v>5.10963369085116</v>
+        <v>6.85148511145698</v>
       </c>
       <c r="H99" t="n">
-        <v>5000</v>
+        <v>525.998504041046</v>
       </c>
       <c r="I99" t="n">
         <v>5.10963369085116</v>
@@ -3840,13 +3975,14 @@
       <c r="K99" t="n">
         <v>0.548488020390718</v>
       </c>
+      <c r="L99"/>
     </row>
     <row r="100">
       <c r="A100" t="n">
         <v>99</v>
       </c>
       <c r="B100" t="n">
-        <v>14.2679872</v>
+        <v>14.2444117536288</v>
       </c>
       <c r="C100" t="n">
         <v>32.8925798881951</v>
@@ -3855,16 +3991,16 @@
         <v>32.5991696301406</v>
       </c>
       <c r="E100" t="n">
-        <v>5000</v>
+        <v>525.998504041046</v>
       </c>
       <c r="F100" t="n">
         <v>3.60715613033392</v>
       </c>
       <c r="G100" t="n">
-        <v>5.10963369085116</v>
+        <v>6.85148511145698</v>
       </c>
       <c r="H100" t="n">
-        <v>5000</v>
+        <v>525.998504041046</v>
       </c>
       <c r="I100" t="n">
         <v>5.10963369085116</v>
@@ -3875,13 +4011,14 @@
       <c r="K100" t="n">
         <v>0.541657219677038</v>
       </c>
+      <c r="L100"/>
     </row>
     <row r="101">
       <c r="A101" t="n">
         <v>100</v>
       </c>
       <c r="B101" t="n">
-        <v>14.23264</v>
+        <v>14.2065110130099</v>
       </c>
       <c r="C101" t="n">
         <v>32.9803321264109</v>
@@ -3890,16 +4027,16 @@
         <v>32.6860154626982</v>
       </c>
       <c r="E101" t="n">
-        <v>5000</v>
+        <v>525.998504041046</v>
       </c>
       <c r="F101" t="n">
         <v>3.60715613033392</v>
       </c>
       <c r="G101" t="n">
-        <v>5.10963369085116</v>
+        <v>6.85148511145698</v>
       </c>
       <c r="H101" t="n">
-        <v>5000</v>
+        <v>524.098230984879</v>
       </c>
       <c r="I101" t="n">
         <v>5.10963369085116</v>
@@ -3909,6 +4046,9 @@
       </c>
       <c r="K101" t="n">
         <v>0.53501513709981</v>
+      </c>
+      <c r="L101" t="n">
+        <v>1.90027305616695</v>
       </c>
     </row>
     <row r="102">
@@ -3916,7 +4056,7 @@
         <v>101</v>
       </c>
       <c r="B102" t="n">
-        <v>14.1972928</v>
+        <v>14.1954788554404</v>
       </c>
       <c r="C102" t="n">
         <v>33.0657454167625</v>
@@ -3925,16 +4065,16 @@
         <v>32.7705461413859</v>
       </c>
       <c r="E102" t="n">
-        <v>5000</v>
+        <v>524.098230984879</v>
       </c>
       <c r="F102" t="n">
         <v>3.60715613033392</v>
       </c>
       <c r="G102" t="n">
-        <v>5.10963369085116</v>
+        <v>6.85148511145698</v>
       </c>
       <c r="H102" t="n">
-        <v>5000</v>
+        <v>524.098230984879</v>
       </c>
       <c r="I102" t="n">
         <v>5.10963369085116</v>
@@ -3945,6 +4085,7 @@
       <c r="K102" t="n">
         <v>0.528556515331397</v>
       </c>
+      <c r="L102"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>